<commit_message>
labview miltiple unit selection
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec_v4.xlsx
+++ b/1-SystemDocs/System_spec_v4.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="781">
   <si>
     <t>ETH*</t>
   </si>
@@ -2429,6 +2429,18 @@
   </si>
   <si>
     <t>Electrochemical sensor configuration readback failed at A3.2</t>
+  </si>
+  <si>
+    <t>Fan control - implement control from Labview for Fan header</t>
+  </si>
+  <si>
+    <t>Create high level system document, documenting the project</t>
+  </si>
+  <si>
+    <t>add configutaion set to log</t>
+  </si>
+  <si>
+    <t>array for unit selection, switch for single and multiple config</t>
   </si>
 </sst>
 </file>
@@ -3895,11 +3907,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="343293592"/>
-        <c:axId val="343353544"/>
+        <c:axId val="372743552"/>
+        <c:axId val="372743936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="343293592"/>
+        <c:axId val="372743552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3944,12 +3956,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343353544"/>
+        <c:crossAx val="372743936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="343353544"/>
+        <c:axId val="372743936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1400"/>
@@ -4008,7 +4020,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343293592"/>
+        <c:crossAx val="372743552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4724,7 +4736,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12379,10 +12391,10 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12878,6 +12890,26 @@
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>740</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update of conf. sets
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec_v4.xlsx
+++ b/1-SystemDocs/System_spec_v4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="12960" windowHeight="11760" firstSheet="10" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="12960" windowHeight="11760" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="777">
   <si>
     <t>ETH*</t>
   </si>
@@ -2389,18 +2389,6 @@
     <t>NO-AE plugged</t>
   </si>
   <si>
-    <t>0b00010000</t>
-  </si>
-  <si>
-    <t>0b00100000</t>
-  </si>
-  <si>
-    <t>0b00100001</t>
-  </si>
-  <si>
-    <t>0b00110001</t>
-  </si>
-  <si>
     <t>Electrochemical sensor configuration readback failed at A1.0</t>
   </si>
   <si>
@@ -2447,7 +2435,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2585,6 +2573,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="17">
@@ -3021,7 +3015,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3344,11 +3338,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3356,6 +3346,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3403,6 +3397,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3418,29 +3436,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3907,11 +3904,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="372743552"/>
-        <c:axId val="372743936"/>
+        <c:axId val="366050544"/>
+        <c:axId val="329149320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="372743552"/>
+        <c:axId val="366050544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3956,12 +3953,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="372743936"/>
+        <c:crossAx val="329149320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="372743936"/>
+        <c:axId val="329149320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1400"/>
@@ -4020,7 +4017,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="372743552"/>
+        <c:crossAx val="366050544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4736,7 +4733,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5679,7 +5676,7 @@
   <dimension ref="B1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8824,8 +8821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V63"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8852,19 +8849,19 @@
       </c>
     </row>
     <row r="3" spans="2:22" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="219" t="s">
+      <c r="B3" s="209" t="s">
         <v>537</v>
       </c>
-      <c r="C3" s="219"/>
-      <c r="D3" s="219"/>
-      <c r="E3" s="219"/>
-      <c r="F3" s="219"/>
-      <c r="G3" s="219"/>
-      <c r="H3" s="219"/>
-      <c r="I3" s="219"/>
-      <c r="J3" s="219"/>
-      <c r="K3" s="219"/>
-      <c r="L3" s="219"/>
+      <c r="C3" s="209"/>
+      <c r="D3" s="209"/>
+      <c r="E3" s="209"/>
+      <c r="F3" s="209"/>
+      <c r="G3" s="209"/>
+      <c r="H3" s="209"/>
+      <c r="I3" s="209"/>
+      <c r="J3" s="209"/>
+      <c r="K3" s="209"/>
+      <c r="L3" s="209"/>
       <c r="M3" s="129"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
@@ -9003,16 +9000,16 @@
       <c r="B10" s="151" t="s">
         <v>636</v>
       </c>
-      <c r="C10" s="220" t="s">
+      <c r="C10" s="210" t="s">
         <v>643</v>
       </c>
-      <c r="D10" s="220"/>
-      <c r="E10" s="220"/>
-      <c r="F10" s="220"/>
-      <c r="G10" s="220"/>
-      <c r="H10" s="220"/>
-      <c r="I10" s="220"/>
-      <c r="J10" s="221"/>
+      <c r="D10" s="210"/>
+      <c r="E10" s="210"/>
+      <c r="F10" s="210"/>
+      <c r="G10" s="210"/>
+      <c r="H10" s="210"/>
+      <c r="I10" s="210"/>
+      <c r="J10" s="211"/>
       <c r="T10" s="22">
         <v>9</v>
       </c>
@@ -9027,16 +9024,16 @@
       <c r="B11" s="151" t="s">
         <v>642</v>
       </c>
-      <c r="C11" s="220" t="s">
+      <c r="C11" s="210" t="s">
         <v>645</v>
       </c>
-      <c r="D11" s="220"/>
-      <c r="E11" s="220"/>
-      <c r="F11" s="220"/>
-      <c r="G11" s="220"/>
-      <c r="H11" s="220"/>
-      <c r="I11" s="220"/>
-      <c r="J11" s="221"/>
+      <c r="D11" s="210"/>
+      <c r="E11" s="210"/>
+      <c r="F11" s="210"/>
+      <c r="G11" s="210"/>
+      <c r="H11" s="210"/>
+      <c r="I11" s="210"/>
+      <c r="J11" s="211"/>
       <c r="T11" s="24" t="s">
         <v>102</v>
       </c>
@@ -9051,16 +9048,16 @@
       <c r="B12" s="144" t="s">
         <v>641</v>
       </c>
-      <c r="C12" s="222" t="s">
+      <c r="C12" s="212" t="s">
         <v>644</v>
       </c>
-      <c r="D12" s="222"/>
-      <c r="E12" s="222"/>
-      <c r="F12" s="222"/>
-      <c r="G12" s="222"/>
-      <c r="H12" s="222"/>
-      <c r="I12" s="222"/>
-      <c r="J12" s="223"/>
+      <c r="D12" s="212"/>
+      <c r="E12" s="212"/>
+      <c r="F12" s="212"/>
+      <c r="G12" s="212"/>
+      <c r="H12" s="212"/>
+      <c r="I12" s="212"/>
+      <c r="J12" s="213"/>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -9073,26 +9070,26 @@
       </c>
       <c r="C15" s="159"/>
       <c r="D15" s="159"/>
-      <c r="E15" s="212" t="s">
+      <c r="E15" s="218" t="s">
         <v>681</v>
       </c>
-      <c r="F15" s="213"/>
-      <c r="G15" s="214"/>
+      <c r="F15" s="219"/>
+      <c r="G15" s="220"/>
       <c r="H15" s="159"/>
       <c r="I15" s="159"/>
       <c r="J15" s="160"/>
-      <c r="L15" s="215" t="s">
+      <c r="L15" s="221" t="s">
         <v>706</v>
       </c>
-      <c r="M15" s="215"/>
-      <c r="N15" s="215"/>
-      <c r="O15" s="215"/>
-      <c r="P15" s="215"/>
-      <c r="Q15" s="215"/>
-      <c r="R15" s="215"/>
+      <c r="M15" s="221"/>
+      <c r="N15" s="221"/>
+      <c r="O15" s="221"/>
+      <c r="P15" s="221"/>
+      <c r="Q15" s="221"/>
+      <c r="R15" s="221"/>
     </row>
     <row r="16" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="216">
+      <c r="B16" s="214">
         <v>1</v>
       </c>
       <c r="C16" s="28" t="s">
@@ -9143,13 +9140,13 @@
       <c r="S16" s="182" t="s">
         <v>758</v>
       </c>
-      <c r="U16" s="211" t="s">
+      <c r="U16" s="217" t="s">
         <v>659</v>
       </c>
-      <c r="V16" s="211"/>
+      <c r="V16" s="217"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="217"/>
+      <c r="B17" s="215"/>
       <c r="C17" s="31" t="s">
         <v>428</v>
       </c>
@@ -9211,7 +9208,7 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="217"/>
+      <c r="B18" s="215"/>
       <c r="C18" s="31" t="s">
         <v>433</v>
       </c>
@@ -9232,7 +9229,7 @@
       </c>
     </row>
     <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="218"/>
+      <c r="B19" s="216"/>
       <c r="C19" s="35" t="s">
         <v>648</v>
       </c>
@@ -9251,7 +9248,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="216">
+      <c r="B20" s="214">
         <v>2</v>
       </c>
       <c r="C20" s="28" t="s">
@@ -9286,7 +9283,7 @@
       </c>
     </row>
     <row r="21" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="217"/>
+      <c r="B21" s="215"/>
       <c r="C21" s="31" t="s">
         <v>424</v>
       </c>
@@ -9356,7 +9353,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="217"/>
+      <c r="B22" s="215"/>
       <c r="C22" s="31" t="s">
         <v>425</v>
       </c>
@@ -9426,7 +9423,7 @@
       </c>
     </row>
     <row r="23" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="217"/>
+      <c r="B23" s="215"/>
       <c r="C23" s="31" t="s">
         <v>426</v>
       </c>
@@ -9496,7 +9493,7 @@
       </c>
     </row>
     <row r="24" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="217"/>
+      <c r="B24" s="215"/>
       <c r="C24" s="81" t="s">
         <v>427</v>
       </c>
@@ -9566,7 +9563,7 @@
       </c>
     </row>
     <row r="25" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="217"/>
+      <c r="B25" s="215"/>
       <c r="C25" s="31" t="s">
         <v>428</v>
       </c>
@@ -9636,7 +9633,7 @@
       </c>
     </row>
     <row r="26" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="217"/>
+      <c r="B26" s="215"/>
       <c r="C26" s="31" t="s">
         <v>429</v>
       </c>
@@ -9703,7 +9700,7 @@
       </c>
     </row>
     <row r="27" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="217"/>
+      <c r="B27" s="215"/>
       <c r="C27" s="81" t="s">
         <v>430</v>
       </c>
@@ -9770,7 +9767,7 @@
       </c>
     </row>
     <row r="28" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="217"/>
+      <c r="B28" s="215"/>
       <c r="C28" s="31" t="s">
         <v>431</v>
       </c>
@@ -9799,7 +9796,7 @@
       </c>
     </row>
     <row r="29" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="217"/>
+      <c r="B29" s="215"/>
       <c r="C29" s="31" t="s">
         <v>433</v>
       </c>
@@ -9828,7 +9825,7 @@
       </c>
     </row>
     <row r="30" spans="2:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="218"/>
+      <c r="B30" s="216"/>
       <c r="C30" s="35" t="s">
         <v>434</v>
       </c>
@@ -9857,81 +9854,82 @@
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="137"/>
-      <c r="H31" s="137"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
+      <c r="B31" s="214">
+        <v>3</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="E31" s="164" t="s">
+        <v>560</v>
+      </c>
+      <c r="F31" s="164" t="s">
+        <v>561</v>
+      </c>
+      <c r="G31" s="164" t="s">
+        <v>562</v>
+      </c>
+      <c r="H31" s="155" t="s">
+        <v>560</v>
+      </c>
+      <c r="I31" s="155" t="s">
+        <v>561</v>
+      </c>
+      <c r="J31" s="156" t="s">
+        <v>562</v>
+      </c>
       <c r="K31" s="10"/>
       <c r="L31" s="137"/>
       <c r="M31" s="137"/>
       <c r="N31" s="137"/>
       <c r="O31" s="137"/>
       <c r="P31" s="137"/>
-      <c r="Q31" s="195"/>
+      <c r="Q31" s="191"/>
       <c r="R31" s="137"/>
       <c r="U31" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
+      <c r="B32" s="215"/>
+      <c r="C32" s="31" t="s">
+        <v>424</v>
+      </c>
+      <c r="D32" s="81" t="s">
+        <v>651</v>
+      </c>
       <c r="E32" s="166" t="s">
-        <v>763</v>
+        <v>708</v>
       </c>
       <c r="F32" s="166" t="s">
-        <v>764</v>
+        <v>563</v>
       </c>
       <c r="G32" s="165" t="s">
         <v>583</v>
       </c>
       <c r="H32" s="157" t="str">
-        <f t="shared" ref="H32" si="13">CONCATENATE("0x",BIN2HEX(RIGHT(E32,LEN(E32)-2),2))</f>
-        <v>0x10</v>
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(E32,LEN(E32)-2),2))</f>
+        <v>0x18</v>
       </c>
       <c r="I32" s="157" t="str">
-        <f t="shared" ref="I32" si="14">CONCATENATE("0x",BIN2HEX(RIGHT(F32,LEN(F32)-2),2))</f>
-        <v>0x20</v>
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(F32,LEN(F32)-2),2))</f>
+        <v>0x00</v>
       </c>
       <c r="J32" s="158" t="str">
-        <f t="shared" ref="J32" si="15">CONCATENATE("0x",BIN2HEX(RIGHT(G32,LEN(G32)-2),2))</f>
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(G32,LEN(G32)-2),2))</f>
         <v>0x03</v>
       </c>
       <c r="K32" s="10"/>
-      <c r="L32" s="11" t="str">
-        <f t="shared" ref="L32" si="16">INDEX($V$18:$V$25,MATCH(LEFT(RIGHT(E32,LEN(E32)-2-3),3),$U$18:$U$25,0))</f>
-        <v>14k</v>
-      </c>
-      <c r="M32" s="11" t="str">
-        <f t="shared" ref="M32" si="17">INDEX($V$27:$V$30,MATCH(LEFT(RIGHT(E32,LEN(E32)-2-6),2),$U$27:$U$30,0))</f>
-        <v>10R</v>
-      </c>
-      <c r="N32" s="11" t="str">
-        <f t="shared" ref="N32" si="18">INDEX($V$32:$V$33,MATCH(LEFT(RIGHT(F32,LEN(F32)-2),1),$U$32:$U$33,0))</f>
-        <v>VDD</v>
-      </c>
-      <c r="O32" s="11" t="str">
-        <f t="shared" ref="O32" si="19">INDEX($V$35:$V$38,MATCH(LEFT(RIGHT(F32,LEN(F32)-2-1),2),$U$35:$U$38,0))</f>
-        <v>50%</v>
-      </c>
-      <c r="P32" s="11" t="str">
-        <f t="shared" ref="P32" si="20">INDEX($V$40:$V$41,MATCH(LEFT(RIGHT(F32,LEN(F32)-2-3),1),$U$40:$U$41,0))</f>
-        <v>NEG</v>
-      </c>
-      <c r="Q32" s="154">
-        <f t="shared" ref="Q32" si="21">INDEX($V$43:$V$56,MATCH(LEFT(RIGHT(F32,LEN(F32)-2-4),4),$U$43:$U$56,0))</f>
-        <v>0</v>
-      </c>
-      <c r="R32" s="11" t="str">
-        <f t="shared" ref="R32" si="22">INDEX($V$58:$V$63,MATCH(LEFT(RIGHT(G32,LEN(G32)-2-5),3),$U$58:$U$63,0))</f>
-        <v>3-lead amperometric</v>
-      </c>
+      <c r="L32" s="137"/>
+      <c r="M32" s="137"/>
+      <c r="N32" s="137"/>
+      <c r="O32" s="137"/>
+      <c r="P32" s="137"/>
+      <c r="Q32" s="191"/>
+      <c r="R32" s="137"/>
       <c r="U32" s="153" t="s">
         <v>677</v>
       </c>
@@ -9940,59 +9938,42 @@
       </c>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
+      <c r="B33" s="215"/>
+      <c r="C33" s="31" t="s">
+        <v>425</v>
+      </c>
+      <c r="D33" s="87" t="s">
+        <v>223</v>
+      </c>
       <c r="E33" s="166" t="s">
-        <v>763</v>
+        <v>735</v>
       </c>
       <c r="F33" s="166" t="s">
-        <v>765</v>
+        <v>564</v>
       </c>
       <c r="G33" s="165" t="s">
         <v>583</v>
       </c>
       <c r="H33" s="157" t="str">
-        <f t="shared" ref="H33" si="23">CONCATENATE("0x",BIN2HEX(RIGHT(E33,LEN(E33)-2),2))</f>
-        <v>0x10</v>
+        <f t="shared" ref="H33:H37" si="13">CONCATENATE("0x",BIN2HEX(RIGHT(E33,LEN(E33)-2),2))</f>
+        <v>0x0E</v>
       </c>
       <c r="I33" s="157" t="str">
-        <f t="shared" ref="I33" si="24">CONCATENATE("0x",BIN2HEX(RIGHT(F33,LEN(F33)-2),2))</f>
-        <v>0x21</v>
+        <f t="shared" ref="I33:I37" si="14">CONCATENATE("0x",BIN2HEX(RIGHT(F33,LEN(F33)-2),2))</f>
+        <v>0x40</v>
       </c>
       <c r="J33" s="158" t="str">
-        <f t="shared" ref="J33" si="25">CONCATENATE("0x",BIN2HEX(RIGHT(G33,LEN(G33)-2),2))</f>
+        <f t="shared" ref="J33:J37" si="15">CONCATENATE("0x",BIN2HEX(RIGHT(G33,LEN(G33)-2),2))</f>
         <v>0x03</v>
       </c>
       <c r="K33" s="10"/>
-      <c r="L33" s="11" t="str">
-        <f t="shared" ref="L33" si="26">INDEX($V$18:$V$25,MATCH(LEFT(RIGHT(E33,LEN(E33)-2-3),3),$U$18:$U$25,0))</f>
-        <v>14k</v>
-      </c>
-      <c r="M33" s="11" t="str">
-        <f t="shared" ref="M33" si="27">INDEX($V$27:$V$30,MATCH(LEFT(RIGHT(E33,LEN(E33)-2-6),2),$U$27:$U$30,0))</f>
-        <v>10R</v>
-      </c>
-      <c r="N33" s="11" t="str">
-        <f t="shared" ref="N33" si="28">INDEX($V$32:$V$33,MATCH(LEFT(RIGHT(F33,LEN(F33)-2),1),$U$32:$U$33,0))</f>
-        <v>VDD</v>
-      </c>
-      <c r="O33" s="11" t="str">
-        <f t="shared" ref="O33" si="29">INDEX($V$35:$V$38,MATCH(LEFT(RIGHT(F33,LEN(F33)-2-1),2),$U$35:$U$38,0))</f>
-        <v>50%</v>
-      </c>
-      <c r="P33" s="11" t="str">
-        <f t="shared" ref="P33" si="30">INDEX($V$40:$V$41,MATCH(LEFT(RIGHT(F33,LEN(F33)-2-3),1),$U$40:$U$41,0))</f>
-        <v>NEG</v>
-      </c>
-      <c r="Q33" s="154">
-        <f t="shared" ref="Q33" si="31">INDEX($V$43:$V$56,MATCH(LEFT(RIGHT(F33,LEN(F33)-2-4),4),$U$43:$U$56,0))</f>
-        <v>0.01</v>
-      </c>
-      <c r="R33" s="11" t="str">
-        <f t="shared" ref="R33" si="32">INDEX($V$58:$V$63,MATCH(LEFT(RIGHT(G33,LEN(G33)-2-5),3),$U$58:$U$63,0))</f>
-        <v>3-lead amperometric</v>
-      </c>
+      <c r="L33" s="137"/>
+      <c r="M33" s="137"/>
+      <c r="N33" s="137"/>
+      <c r="O33" s="137"/>
+      <c r="P33" s="137"/>
+      <c r="Q33" s="191"/>
+      <c r="R33" s="137"/>
       <c r="U33" s="153" t="s">
         <v>678</v>
       </c>
@@ -10001,76 +9982,78 @@
       </c>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
+      <c r="B34" s="215"/>
+      <c r="C34" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>545</v>
+      </c>
       <c r="E34" s="166" t="s">
-        <v>763</v>
+        <v>709</v>
       </c>
       <c r="F34" s="166" t="s">
-        <v>766</v>
+        <v>564</v>
       </c>
       <c r="G34" s="165" t="s">
         <v>583</v>
       </c>
       <c r="H34" s="157" t="str">
-        <f t="shared" ref="H34" si="33">CONCATENATE("0x",BIN2HEX(RIGHT(E34,LEN(E34)-2),2))</f>
-        <v>0x10</v>
+        <f t="shared" si="13"/>
+        <v>0x15</v>
       </c>
       <c r="I34" s="157" t="str">
-        <f t="shared" ref="I34" si="34">CONCATENATE("0x",BIN2HEX(RIGHT(F34,LEN(F34)-2),2))</f>
-        <v>0x31</v>
+        <f t="shared" si="14"/>
+        <v>0x40</v>
       </c>
       <c r="J34" s="158" t="str">
-        <f t="shared" ref="J34" si="35">CONCATENATE("0x",BIN2HEX(RIGHT(G34,LEN(G34)-2),2))</f>
+        <f t="shared" si="15"/>
         <v>0x03</v>
       </c>
       <c r="K34" s="10"/>
-      <c r="L34" s="11" t="str">
-        <f t="shared" ref="L34" si="36">INDEX($V$18:$V$25,MATCH(LEFT(RIGHT(E34,LEN(E34)-2-3),3),$U$18:$U$25,0))</f>
-        <v>14k</v>
-      </c>
-      <c r="M34" s="11" t="str">
-        <f t="shared" ref="M34" si="37">INDEX($V$27:$V$30,MATCH(LEFT(RIGHT(E34,LEN(E34)-2-6),2),$U$27:$U$30,0))</f>
-        <v>10R</v>
-      </c>
-      <c r="N34" s="11" t="str">
-        <f t="shared" ref="N34" si="38">INDEX($V$32:$V$33,MATCH(LEFT(RIGHT(F34,LEN(F34)-2),1),$U$32:$U$33,0))</f>
-        <v>VDD</v>
-      </c>
-      <c r="O34" s="11" t="str">
-        <f t="shared" ref="O34" si="39">INDEX($V$35:$V$38,MATCH(LEFT(RIGHT(F34,LEN(F34)-2-1),2),$U$35:$U$38,0))</f>
-        <v>50%</v>
-      </c>
-      <c r="P34" s="11" t="str">
-        <f t="shared" ref="P34" si="40">INDEX($V$40:$V$41,MATCH(LEFT(RIGHT(F34,LEN(F34)-2-3),1),$U$40:$U$41,0))</f>
-        <v>POS</v>
-      </c>
-      <c r="Q34" s="154">
-        <f t="shared" ref="Q34" si="41">INDEX($V$43:$V$56,MATCH(LEFT(RIGHT(F34,LEN(F34)-2-4),4),$U$43:$U$56,0))</f>
-        <v>0.01</v>
-      </c>
-      <c r="R34" s="11" t="str">
-        <f t="shared" ref="R34" si="42">INDEX($V$58:$V$63,MATCH(LEFT(RIGHT(G34,LEN(G34)-2-5),3),$U$58:$U$63,0))</f>
-        <v>3-lead amperometric</v>
-      </c>
+      <c r="L34" s="137"/>
+      <c r="M34" s="137"/>
+      <c r="N34" s="137"/>
+      <c r="O34" s="137"/>
+      <c r="P34" s="137"/>
+      <c r="Q34" s="191"/>
+      <c r="R34" s="137"/>
       <c r="U34" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="195"/>
-      <c r="F35" s="195"/>
-      <c r="G35" s="194"/>
-      <c r="H35" s="194"/>
-      <c r="I35" s="194"/>
-      <c r="J35" s="194"/>
-      <c r="K35" s="194"/>
-      <c r="L35" s="194"/>
-      <c r="M35" s="194"/>
+      <c r="B35" s="215"/>
+      <c r="C35" s="81" t="s">
+        <v>427</v>
+      </c>
+      <c r="D35" s="87" t="s">
+        <v>542</v>
+      </c>
+      <c r="E35" s="168" t="s">
+        <v>750</v>
+      </c>
+      <c r="F35" s="168" t="s">
+        <v>710</v>
+      </c>
+      <c r="G35" s="176" t="s">
+        <v>583</v>
+      </c>
+      <c r="H35" s="177" t="str">
+        <f t="shared" si="13"/>
+        <v>0x11</v>
+      </c>
+      <c r="I35" s="177" t="str">
+        <f t="shared" si="14"/>
+        <v>0x14</v>
+      </c>
+      <c r="J35" s="178" t="str">
+        <f t="shared" si="15"/>
+        <v>0x03</v>
+      </c>
+      <c r="K35" s="190"/>
+      <c r="L35" s="190"/>
+      <c r="M35" s="190"/>
       <c r="N35" s="10"/>
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
@@ -10084,15 +10067,34 @@
       </c>
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="137"/>
-      <c r="F36" s="137"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
+      <c r="B36" s="215"/>
+      <c r="C36" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="D36" s="87" t="s">
+        <v>548</v>
+      </c>
+      <c r="E36" s="166" t="s">
+        <v>753</v>
+      </c>
+      <c r="F36" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G36" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H36" s="157" t="str">
+        <f t="shared" si="13"/>
+        <v>0x19</v>
+      </c>
+      <c r="I36" s="157" t="str">
+        <f t="shared" si="14"/>
+        <v>0x00</v>
+      </c>
+      <c r="J36" s="158" t="str">
+        <f t="shared" si="15"/>
+        <v>0x03</v>
+      </c>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
@@ -10109,18 +10111,37 @@
       </c>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
+      <c r="B37" s="215"/>
+      <c r="C37" s="31" t="s">
+        <v>429</v>
+      </c>
+      <c r="D37" s="87" t="s">
+        <v>547</v>
+      </c>
+      <c r="E37" s="166" t="s">
+        <v>753</v>
+      </c>
+      <c r="F37" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G37" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H37" s="157" t="str">
+        <f t="shared" si="13"/>
+        <v>0x19</v>
+      </c>
+      <c r="I37" s="157" t="str">
+        <f t="shared" si="14"/>
+        <v>0x00</v>
+      </c>
+      <c r="J37" s="158" t="str">
+        <f t="shared" si="15"/>
+        <v>0x03</v>
+      </c>
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
+      <c r="M37" s="192"/>
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
       <c r="P37" s="10"/>
@@ -10134,15 +10155,21 @@
       </c>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
+      <c r="B38" s="215"/>
+      <c r="C38" s="81" t="s">
+        <v>430</v>
+      </c>
+      <c r="D38" s="87" t="s">
+        <v>759</v>
+      </c>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
+      <c r="G38" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H38" s="157"/>
+      <c r="I38" s="157"/>
+      <c r="J38" s="158"/>
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
@@ -10159,17 +10186,23 @@
       </c>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
+      <c r="B39" s="215"/>
+      <c r="C39" s="31" t="s">
+        <v>431</v>
+      </c>
+      <c r="D39" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E39" s="137"/>
+      <c r="F39" s="137"/>
+      <c r="G39" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H39" s="157"/>
+      <c r="I39" s="157"/>
+      <c r="J39" s="158"/>
       <c r="K39" s="10"/>
-      <c r="L39" s="194"/>
+      <c r="L39" s="190"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
       <c r="O39" s="10"/>
@@ -10181,17 +10214,21 @@
       </c>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
+      <c r="B40" s="215"/>
+      <c r="C40" s="31" t="s">
+        <v>433</v>
+      </c>
+      <c r="D40" s="166" t="s">
+        <v>649</v>
+      </c>
+      <c r="E40" s="166"/>
+      <c r="F40" s="166"/>
+      <c r="G40" s="166"/>
+      <c r="H40" s="157"/>
+      <c r="I40" s="157"/>
+      <c r="J40" s="158"/>
       <c r="K40" s="10"/>
-      <c r="L40" s="194"/>
+      <c r="L40" s="190"/>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
@@ -10205,18 +10242,24 @@
         <v>687</v>
       </c>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="193"/>
+    <row r="41" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="216"/>
+      <c r="C41" s="35" t="s">
+        <v>434</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>759</v>
+      </c>
       <c r="E41" s="193"/>
       <c r="F41" s="193"/>
-      <c r="G41" s="193"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="194"/>
-      <c r="L41" s="194"/>
+      <c r="G41" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H41" s="162"/>
+      <c r="I41" s="162"/>
+      <c r="J41" s="163"/>
+      <c r="K41" s="190"/>
+      <c r="L41" s="190"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
       <c r="O41" s="10"/>
@@ -10231,17 +10274,35 @@
       </c>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
+      <c r="B42" s="214">
+        <v>4</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="E42" s="164" t="s">
+        <v>560</v>
+      </c>
+      <c r="F42" s="164" t="s">
+        <v>561</v>
+      </c>
+      <c r="G42" s="164" t="s">
+        <v>562</v>
+      </c>
+      <c r="H42" s="155" t="s">
+        <v>560</v>
+      </c>
+      <c r="I42" s="155" t="s">
+        <v>561</v>
+      </c>
+      <c r="J42" s="156" t="s">
+        <v>562</v>
+      </c>
       <c r="K42" s="10"/>
-      <c r="L42" s="194"/>
+      <c r="L42" s="190"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
       <c r="O42" s="10"/>
@@ -10253,15 +10314,34 @@
       </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B43" s="183"/>
-      <c r="C43" s="183"/>
-      <c r="D43" s="183"/>
-      <c r="E43" s="183"/>
-      <c r="F43" s="183"/>
-      <c r="G43" s="183"/>
-      <c r="H43" s="183"/>
-      <c r="I43" s="183"/>
-      <c r="J43" s="183"/>
+      <c r="B43" s="215"/>
+      <c r="C43" s="31" t="s">
+        <v>424</v>
+      </c>
+      <c r="D43" s="31" t="s">
+        <v>651</v>
+      </c>
+      <c r="E43" s="166" t="s">
+        <v>708</v>
+      </c>
+      <c r="F43" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G43" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H43" s="157" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(E43,LEN(E43)-2),2))</f>
+        <v>0x18</v>
+      </c>
+      <c r="I43" s="157" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(F43,LEN(F43)-2),2))</f>
+        <v>0x00</v>
+      </c>
+      <c r="J43" s="158" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(G43,LEN(G43)-2),2))</f>
+        <v>0x03</v>
+      </c>
       <c r="K43" s="183"/>
       <c r="L43" s="183"/>
       <c r="M43" s="183"/>
@@ -10278,15 +10358,34 @@
       </c>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B44" s="183"/>
-      <c r="C44" s="183"/>
-      <c r="D44" s="183"/>
-      <c r="E44" s="183"/>
-      <c r="F44" s="183"/>
-      <c r="G44" s="183"/>
-      <c r="H44" s="183"/>
-      <c r="I44" s="183"/>
-      <c r="J44" s="183"/>
+      <c r="B44" s="215"/>
+      <c r="C44" s="31" t="s">
+        <v>425</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E44" s="166" t="s">
+        <v>735</v>
+      </c>
+      <c r="F44" s="166" t="s">
+        <v>564</v>
+      </c>
+      <c r="G44" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H44" s="157" t="str">
+        <f t="shared" ref="H44" si="16">CONCATENATE("0x",BIN2HEX(RIGHT(E44,LEN(E44)-2),2))</f>
+        <v>0x0E</v>
+      </c>
+      <c r="I44" s="157" t="str">
+        <f t="shared" ref="I44" si="17">CONCATENATE("0x",BIN2HEX(RIGHT(F44,LEN(F44)-2),2))</f>
+        <v>0x40</v>
+      </c>
+      <c r="J44" s="158" t="str">
+        <f t="shared" ref="J44" si="18">CONCATENATE("0x",BIN2HEX(RIGHT(G44,LEN(G44)-2),2))</f>
+        <v>0x03</v>
+      </c>
       <c r="K44" s="183"/>
       <c r="L44" s="183"/>
       <c r="M44" s="183"/>
@@ -10303,15 +10402,21 @@
       </c>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B45" s="183"/>
-      <c r="C45" s="183"/>
-      <c r="D45" s="183"/>
-      <c r="E45" s="183"/>
-      <c r="F45" s="183"/>
-      <c r="G45" s="183"/>
-      <c r="H45" s="183"/>
-      <c r="I45" s="183"/>
-      <c r="J45" s="183"/>
+      <c r="B45" s="215"/>
+      <c r="C45" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="D45" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H45" s="157"/>
+      <c r="I45" s="157"/>
+      <c r="J45" s="158"/>
       <c r="K45" s="183"/>
       <c r="L45" s="183"/>
       <c r="M45" s="183"/>
@@ -10328,15 +10433,21 @@
       </c>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B46" s="183"/>
-      <c r="C46" s="183"/>
-      <c r="D46" s="183"/>
-      <c r="E46" s="183"/>
-      <c r="F46" s="183"/>
-      <c r="G46" s="183"/>
-      <c r="H46" s="183"/>
-      <c r="I46" s="183"/>
-      <c r="J46" s="183"/>
+      <c r="B46" s="215"/>
+      <c r="C46" s="81" t="s">
+        <v>427</v>
+      </c>
+      <c r="D46" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E46" s="87"/>
+      <c r="F46" s="87"/>
+      <c r="G46" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H46" s="177"/>
+      <c r="I46" s="177"/>
+      <c r="J46" s="178"/>
       <c r="K46" s="183"/>
       <c r="L46" s="183"/>
       <c r="M46" s="183"/>
@@ -10353,15 +10464,21 @@
       </c>
     </row>
     <row r="47" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B47" s="183"/>
-      <c r="C47" s="183"/>
-      <c r="D47" s="183"/>
-      <c r="E47" s="183"/>
-      <c r="F47" s="183"/>
-      <c r="G47" s="183"/>
-      <c r="H47" s="183"/>
-      <c r="I47" s="183"/>
-      <c r="J47" s="183"/>
+      <c r="B47" s="215"/>
+      <c r="C47" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="D47" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H47" s="157"/>
+      <c r="I47" s="157"/>
+      <c r="J47" s="158"/>
       <c r="K47" s="183"/>
       <c r="L47" s="183"/>
       <c r="M47" s="183"/>
@@ -10378,20 +10495,26 @@
       </c>
     </row>
     <row r="48" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B48" s="183"/>
-      <c r="C48" s="185"/>
-      <c r="D48" s="185"/>
-      <c r="E48" s="185"/>
-      <c r="F48" s="185"/>
-      <c r="G48" s="185"/>
-      <c r="H48" s="185"/>
-      <c r="I48" s="185"/>
-      <c r="J48" s="185"/>
-      <c r="K48" s="185"/>
-      <c r="L48" s="185"/>
-      <c r="M48" s="185"/>
-      <c r="N48" s="185"/>
-      <c r="O48" s="185"/>
+      <c r="B48" s="215"/>
+      <c r="C48" s="31" t="s">
+        <v>429</v>
+      </c>
+      <c r="D48" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H48" s="157"/>
+      <c r="I48" s="157"/>
+      <c r="J48" s="158"/>
+      <c r="K48" s="184"/>
+      <c r="L48" s="184"/>
+      <c r="M48" s="184"/>
+      <c r="N48" s="184"/>
+      <c r="O48" s="184"/>
       <c r="P48" s="183"/>
       <c r="Q48" s="183"/>
       <c r="R48" s="183"/>
@@ -10403,15 +10526,21 @@
       </c>
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B49" s="183"/>
-      <c r="C49" s="183"/>
-      <c r="D49" s="183"/>
-      <c r="E49" s="183"/>
-      <c r="F49" s="183"/>
-      <c r="G49" s="183"/>
-      <c r="H49" s="183"/>
-      <c r="I49" s="183"/>
-      <c r="J49" s="183"/>
+      <c r="B49" s="215"/>
+      <c r="C49" s="81" t="s">
+        <v>430</v>
+      </c>
+      <c r="D49" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H49" s="157"/>
+      <c r="I49" s="157"/>
+      <c r="J49" s="158"/>
       <c r="K49" s="183"/>
       <c r="L49" s="183"/>
       <c r="M49" s="183"/>
@@ -10428,15 +10557,21 @@
       </c>
     </row>
     <row r="50" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B50" s="183"/>
-      <c r="C50" s="183"/>
-      <c r="D50" s="183"/>
-      <c r="E50" s="183"/>
-      <c r="F50" s="183"/>
-      <c r="G50" s="183"/>
-      <c r="H50" s="183"/>
-      <c r="I50" s="183"/>
-      <c r="J50" s="183"/>
+      <c r="B50" s="215"/>
+      <c r="C50" s="31" t="s">
+        <v>431</v>
+      </c>
+      <c r="D50" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E50" s="137"/>
+      <c r="F50" s="137"/>
+      <c r="G50" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H50" s="157"/>
+      <c r="I50" s="157"/>
+      <c r="J50" s="158"/>
       <c r="K50" s="183"/>
       <c r="L50" s="183"/>
       <c r="M50" s="183"/>
@@ -10453,15 +10588,19 @@
       </c>
     </row>
     <row r="51" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B51" s="183"/>
-      <c r="C51" s="183"/>
-      <c r="D51" s="183"/>
-      <c r="E51" s="185"/>
-      <c r="F51" s="183"/>
-      <c r="G51" s="183"/>
-      <c r="H51" s="183"/>
-      <c r="I51" s="183"/>
-      <c r="J51" s="183"/>
+      <c r="B51" s="215"/>
+      <c r="C51" s="31" t="s">
+        <v>433</v>
+      </c>
+      <c r="D51" s="166" t="s">
+        <v>649</v>
+      </c>
+      <c r="E51" s="166"/>
+      <c r="F51" s="166"/>
+      <c r="G51" s="166"/>
+      <c r="H51" s="157"/>
+      <c r="I51" s="157"/>
+      <c r="J51" s="158"/>
       <c r="K51" s="183"/>
       <c r="L51" s="183"/>
       <c r="M51" s="183"/>
@@ -10477,16 +10616,22 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="52" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B52" s="183"/>
-      <c r="C52" s="183"/>
-      <c r="D52" s="183"/>
-      <c r="E52" s="183"/>
-      <c r="F52" s="183"/>
-      <c r="G52" s="183"/>
-      <c r="H52" s="183"/>
-      <c r="I52" s="183"/>
-      <c r="J52" s="183"/>
+    <row r="52" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="216"/>
+      <c r="C52" s="35" t="s">
+        <v>434</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>759</v>
+      </c>
+      <c r="E52" s="193"/>
+      <c r="F52" s="193"/>
+      <c r="G52" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H52" s="162"/>
+      <c r="I52" s="162"/>
+      <c r="J52" s="163"/>
       <c r="K52" s="183"/>
       <c r="L52" s="183"/>
       <c r="M52" s="183"/>
@@ -10503,15 +10648,33 @@
       </c>
     </row>
     <row r="53" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B53" s="183"/>
-      <c r="C53" s="183"/>
-      <c r="D53" s="183"/>
-      <c r="E53" s="183"/>
-      <c r="F53" s="183"/>
-      <c r="G53" s="183"/>
-      <c r="H53" s="183"/>
-      <c r="I53" s="183"/>
-      <c r="J53" s="183"/>
+      <c r="B53" s="214">
+        <v>5</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="E53" s="164" t="s">
+        <v>560</v>
+      </c>
+      <c r="F53" s="164" t="s">
+        <v>561</v>
+      </c>
+      <c r="G53" s="164" t="s">
+        <v>562</v>
+      </c>
+      <c r="H53" s="155" t="s">
+        <v>560</v>
+      </c>
+      <c r="I53" s="155" t="s">
+        <v>561</v>
+      </c>
+      <c r="J53" s="156" t="s">
+        <v>562</v>
+      </c>
       <c r="K53" s="183"/>
       <c r="L53" s="183"/>
       <c r="M53" s="183"/>
@@ -10528,15 +10691,34 @@
       </c>
     </row>
     <row r="54" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B54" s="183"/>
-      <c r="C54" s="183"/>
-      <c r="D54" s="185"/>
-      <c r="E54" s="186"/>
-      <c r="F54" s="184"/>
-      <c r="G54" s="183"/>
-      <c r="H54" s="183"/>
-      <c r="I54" s="183"/>
-      <c r="J54" s="183"/>
+      <c r="B54" s="215"/>
+      <c r="C54" s="31" t="s">
+        <v>424</v>
+      </c>
+      <c r="D54" s="31" t="s">
+        <v>651</v>
+      </c>
+      <c r="E54" s="166" t="s">
+        <v>708</v>
+      </c>
+      <c r="F54" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G54" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H54" s="157" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(E54,LEN(E54)-2),2))</f>
+        <v>0x18</v>
+      </c>
+      <c r="I54" s="157" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(F54,LEN(F54)-2),2))</f>
+        <v>0x00</v>
+      </c>
+      <c r="J54" s="158" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(G54,LEN(G54)-2),2))</f>
+        <v>0x03</v>
+      </c>
       <c r="K54" s="183"/>
       <c r="L54" s="183"/>
       <c r="M54" s="183"/>
@@ -10553,15 +10735,34 @@
       </c>
     </row>
     <row r="55" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B55" s="183"/>
-      <c r="C55" s="183"/>
-      <c r="D55" s="187"/>
-      <c r="E55" s="188"/>
-      <c r="F55" s="184"/>
-      <c r="G55" s="183"/>
-      <c r="H55" s="183"/>
-      <c r="I55" s="183"/>
-      <c r="J55" s="183"/>
+      <c r="B55" s="215"/>
+      <c r="C55" s="31" t="s">
+        <v>425</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E55" s="166" t="s">
+        <v>735</v>
+      </c>
+      <c r="F55" s="166" t="s">
+        <v>564</v>
+      </c>
+      <c r="G55" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H55" s="157" t="str">
+        <f t="shared" ref="H55" si="19">CONCATENATE("0x",BIN2HEX(RIGHT(E55,LEN(E55)-2),2))</f>
+        <v>0x0E</v>
+      </c>
+      <c r="I55" s="157" t="str">
+        <f t="shared" ref="I55" si="20">CONCATENATE("0x",BIN2HEX(RIGHT(F55,LEN(F55)-2),2))</f>
+        <v>0x40</v>
+      </c>
+      <c r="J55" s="158" t="str">
+        <f t="shared" ref="J55" si="21">CONCATENATE("0x",BIN2HEX(RIGHT(G55,LEN(G55)-2),2))</f>
+        <v>0x03</v>
+      </c>
       <c r="K55" s="183"/>
       <c r="L55" s="183"/>
       <c r="M55" s="183"/>
@@ -10578,15 +10779,34 @@
       </c>
     </row>
     <row r="56" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B56" s="183"/>
-      <c r="C56" s="183"/>
-      <c r="D56" s="187"/>
-      <c r="E56" s="188"/>
-      <c r="F56" s="184"/>
-      <c r="G56" s="183"/>
-      <c r="H56" s="183"/>
-      <c r="I56" s="183"/>
-      <c r="J56" s="183"/>
+      <c r="B56" s="215"/>
+      <c r="C56" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="D56" s="31" t="s">
+        <v>651</v>
+      </c>
+      <c r="E56" s="166" t="s">
+        <v>708</v>
+      </c>
+      <c r="F56" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G56" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H56" s="157" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(E56,LEN(E56)-2),2))</f>
+        <v>0x18</v>
+      </c>
+      <c r="I56" s="157" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(F56,LEN(F56)-2),2))</f>
+        <v>0x00</v>
+      </c>
+      <c r="J56" s="158" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(G56,LEN(G56)-2),2))</f>
+        <v>0x03</v>
+      </c>
       <c r="K56" s="183"/>
       <c r="L56" s="183"/>
       <c r="M56" s="183"/>
@@ -10603,15 +10823,34 @@
       </c>
     </row>
     <row r="57" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B57" s="183"/>
-      <c r="C57" s="183"/>
-      <c r="D57" s="185"/>
-      <c r="E57" s="186"/>
-      <c r="F57" s="184"/>
-      <c r="G57" s="183"/>
-      <c r="H57" s="183"/>
-      <c r="I57" s="183"/>
-      <c r="J57" s="183"/>
+      <c r="B57" s="215"/>
+      <c r="C57" s="81" t="s">
+        <v>427</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E57" s="166" t="s">
+        <v>735</v>
+      </c>
+      <c r="F57" s="166" t="s">
+        <v>564</v>
+      </c>
+      <c r="G57" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H57" s="157" t="str">
+        <f t="shared" ref="H57" si="22">CONCATENATE("0x",BIN2HEX(RIGHT(E57,LEN(E57)-2),2))</f>
+        <v>0x0E</v>
+      </c>
+      <c r="I57" s="157" t="str">
+        <f t="shared" ref="I57" si="23">CONCATENATE("0x",BIN2HEX(RIGHT(F57,LEN(F57)-2),2))</f>
+        <v>0x40</v>
+      </c>
+      <c r="J57" s="158" t="str">
+        <f t="shared" ref="J57" si="24">CONCATENATE("0x",BIN2HEX(RIGHT(G57,LEN(G57)-2),2))</f>
+        <v>0x03</v>
+      </c>
       <c r="K57" s="183"/>
       <c r="L57" s="183"/>
       <c r="M57" s="183"/>
@@ -10625,15 +10864,21 @@
       </c>
     </row>
     <row r="58" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B58" s="183"/>
-      <c r="C58" s="183"/>
-      <c r="D58" s="183"/>
-      <c r="E58" s="183"/>
-      <c r="F58" s="183"/>
-      <c r="G58" s="183"/>
-      <c r="H58" s="183"/>
-      <c r="I58" s="183"/>
-      <c r="J58" s="183"/>
+      <c r="B58" s="215"/>
+      <c r="C58" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="D58" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H58" s="157"/>
+      <c r="I58" s="157"/>
+      <c r="J58" s="158"/>
       <c r="K58" s="183"/>
       <c r="L58" s="183"/>
       <c r="M58" s="183"/>
@@ -10650,15 +10895,21 @@
       </c>
     </row>
     <row r="59" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B59" s="183"/>
-      <c r="C59" s="183"/>
-      <c r="D59" s="183"/>
-      <c r="E59" s="183"/>
-      <c r="F59" s="183"/>
-      <c r="G59" s="183"/>
-      <c r="H59" s="183"/>
-      <c r="I59" s="183"/>
-      <c r="J59" s="183"/>
+      <c r="B59" s="215"/>
+      <c r="C59" s="31" t="s">
+        <v>429</v>
+      </c>
+      <c r="D59" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H59" s="157"/>
+      <c r="I59" s="157"/>
+      <c r="J59" s="158"/>
       <c r="K59" s="183"/>
       <c r="L59" s="183"/>
       <c r="M59" s="183"/>
@@ -10675,6 +10926,21 @@
       </c>
     </row>
     <row r="60" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B60" s="215"/>
+      <c r="C60" s="81" t="s">
+        <v>430</v>
+      </c>
+      <c r="D60" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H60" s="157"/>
+      <c r="I60" s="157"/>
+      <c r="J60" s="158"/>
       <c r="U60" s="153" t="s">
         <v>663</v>
       </c>
@@ -10683,6 +10949,21 @@
       </c>
     </row>
     <row r="61" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B61" s="215"/>
+      <c r="C61" s="31" t="s">
+        <v>431</v>
+      </c>
+      <c r="D61" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E61" s="137"/>
+      <c r="F61" s="137"/>
+      <c r="G61" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H61" s="157"/>
+      <c r="I61" s="157"/>
+      <c r="J61" s="158"/>
       <c r="U61" s="153" t="s">
         <v>666</v>
       </c>
@@ -10691,6 +10972,19 @@
       </c>
     </row>
     <row r="62" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B62" s="215"/>
+      <c r="C62" s="31" t="s">
+        <v>433</v>
+      </c>
+      <c r="D62" s="166" t="s">
+        <v>649</v>
+      </c>
+      <c r="E62" s="166"/>
+      <c r="F62" s="166"/>
+      <c r="G62" s="166"/>
+      <c r="H62" s="157"/>
+      <c r="I62" s="157"/>
+      <c r="J62" s="158"/>
       <c r="U62" s="153" t="s">
         <v>670</v>
       </c>
@@ -10698,7 +10992,22 @@
         <v>704</v>
       </c>
     </row>
-    <row r="63" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="216"/>
+      <c r="C63" s="35" t="s">
+        <v>434</v>
+      </c>
+      <c r="D63" s="35" t="s">
+        <v>759</v>
+      </c>
+      <c r="E63" s="193"/>
+      <c r="F63" s="193"/>
+      <c r="G63" s="222" t="s">
+        <v>563</v>
+      </c>
+      <c r="H63" s="162"/>
+      <c r="I63" s="162"/>
+      <c r="J63" s="163"/>
       <c r="U63" s="153" t="s">
         <v>667</v>
       </c>
@@ -10707,7 +11016,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="B31:B41"/>
+    <mergeCell ref="B42:B52"/>
+    <mergeCell ref="B53:B63"/>
     <mergeCell ref="U16:V16"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="L15:R15"/>
@@ -11611,28 +11923,28 @@
       <c r="A56" s="30"/>
       <c r="B56" s="31"/>
       <c r="C56" s="31"/>
-      <c r="D56" s="189" t="s">
+      <c r="D56" s="185" t="s">
         <v>741</v>
       </c>
-      <c r="E56" s="190"/>
-      <c r="F56" s="190"/>
-      <c r="G56" s="190"/>
-      <c r="H56" s="190">
+      <c r="E56" s="186"/>
+      <c r="F56" s="186"/>
+      <c r="G56" s="186"/>
+      <c r="H56" s="186">
         <v>-9.9000000000000005E-2</v>
       </c>
-      <c r="I56" s="190">
+      <c r="I56" s="186">
         <v>-9.9000000000000005E-2</v>
       </c>
-      <c r="J56" s="190">
+      <c r="J56" s="186">
         <v>0.1</v>
       </c>
-      <c r="K56" s="191">
+      <c r="K56" s="187">
         <v>0.498</v>
       </c>
-      <c r="L56" s="192">
+      <c r="L56" s="188">
         <v>0.29899999999999999</v>
       </c>
-      <c r="M56" s="193">
+      <c r="M56" s="189">
         <v>0.29899999999999999</v>
       </c>
       <c r="N56" s="31"/>
@@ -12114,7 +12426,7 @@
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -12122,7 +12434,7 @@
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -12130,7 +12442,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -12138,7 +12450,7 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -12146,7 +12458,7 @@
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -12154,7 +12466,7 @@
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -12162,7 +12474,7 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -12170,7 +12482,7 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -12178,7 +12490,7 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -12186,7 +12498,7 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
     </row>
   </sheetData>
@@ -12393,9 +12705,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12892,24 +13202,30 @@
         <v>740</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+        <v>775</v>
+      </c>
+      <c r="B67" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>780</v>
+        <v>776</v>
+      </c>
+      <c r="B68" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -14591,16 +14907,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A4" s="196" t="s">
+      <c r="A4" s="194" t="s">
         <v>280</v>
       </c>
-      <c r="B4" s="196"/>
-      <c r="C4" s="196"/>
-      <c r="E4" s="196" t="s">
+      <c r="B4" s="194"/>
+      <c r="C4" s="194"/>
+      <c r="E4" s="194" t="s">
         <v>281</v>
       </c>
-      <c r="F4" s="196"/>
-      <c r="G4" s="196"/>
+      <c r="F4" s="194"/>
+      <c r="G4" s="194"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -14843,16 +15159,16 @@
       </c>
     </row>
     <row r="3" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B3" s="196" t="s">
+      <c r="B3" s="194" t="s">
         <v>292</v>
       </c>
-      <c r="C3" s="196"/>
-      <c r="D3" s="196"/>
-      <c r="H3" s="196" t="s">
+      <c r="C3" s="194"/>
+      <c r="D3" s="194"/>
+      <c r="H3" s="194" t="s">
         <v>293</v>
       </c>
-      <c r="I3" s="196"/>
-      <c r="J3" s="196"/>
+      <c r="I3" s="194"/>
+      <c r="J3" s="194"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -15016,11 +15332,11 @@
       </c>
     </row>
     <row r="22" spans="2:10" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H22" s="197" t="s">
+      <c r="H22" s="195" t="s">
         <v>307</v>
       </c>
-      <c r="I22" s="198"/>
-      <c r="J22" s="199"/>
+      <c r="I22" s="196"/>
+      <c r="J22" s="197"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="27" t="s">
@@ -15030,9 +15346,9 @@
         <v>106</v>
       </c>
       <c r="D23" s="29"/>
-      <c r="H23" s="200"/>
-      <c r="I23" s="201"/>
-      <c r="J23" s="202"/>
+      <c r="H23" s="198"/>
+      <c r="I23" s="199"/>
+      <c r="J23" s="200"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="30">
@@ -15753,11 +16069,11 @@
       <c r="B4" s="86" t="s">
         <v>383</v>
       </c>
-      <c r="I4" s="203" t="s">
+      <c r="I4" s="201" t="s">
         <v>394</v>
       </c>
-      <c r="J4" s="204"/>
-      <c r="K4" s="205"/>
+      <c r="J4" s="202"/>
+      <c r="K4" s="203"/>
     </row>
     <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
@@ -15858,12 +16174,12 @@
       <c r="B8" s="75" t="s">
         <v>384</v>
       </c>
-      <c r="C8" s="208" t="s">
+      <c r="C8" s="206" t="s">
         <v>387</v>
       </c>
-      <c r="D8" s="210"/>
-      <c r="E8" s="210"/>
-      <c r="F8" s="209"/>
+      <c r="D8" s="208"/>
+      <c r="E8" s="208"/>
+      <c r="F8" s="207"/>
       <c r="G8" s="94" t="s">
         <v>388</v>
       </c>
@@ -15873,17 +16189,17 @@
       <c r="I8" s="100" t="s">
         <v>403</v>
       </c>
-      <c r="J8" s="206" t="s">
+      <c r="J8" s="204" t="s">
         <v>397</v>
       </c>
-      <c r="K8" s="207"/>
+      <c r="K8" s="205"/>
       <c r="L8" s="94" t="s">
         <v>389</v>
       </c>
-      <c r="M8" s="206" t="s">
+      <c r="M8" s="204" t="s">
         <v>397</v>
       </c>
-      <c r="N8" s="207"/>
+      <c r="N8" s="205"/>
       <c r="O8" s="91" t="s">
         <v>129</v>
       </c>
@@ -15895,12 +16211,12 @@
       <c r="B9" s="75" t="s">
         <v>386</v>
       </c>
-      <c r="C9" s="208" t="s">
+      <c r="C9" s="206" t="s">
         <v>387</v>
       </c>
-      <c r="D9" s="210"/>
-      <c r="E9" s="210"/>
-      <c r="F9" s="209"/>
+      <c r="D9" s="208"/>
+      <c r="E9" s="208"/>
+      <c r="F9" s="207"/>
       <c r="G9" s="94" t="s">
         <v>393</v>
       </c>
@@ -15910,17 +16226,17 @@
       <c r="I9" s="94" t="s">
         <v>390</v>
       </c>
-      <c r="J9" s="208" t="s">
+      <c r="J9" s="206" t="s">
         <v>565</v>
       </c>
-      <c r="K9" s="209"/>
+      <c r="K9" s="207"/>
       <c r="L9" s="94" t="s">
         <v>398</v>
       </c>
-      <c r="M9" s="208" t="s">
+      <c r="M9" s="206" t="s">
         <v>566</v>
       </c>
-      <c r="N9" s="209"/>
+      <c r="N9" s="207"/>
       <c r="O9" s="91" t="s">
         <v>129</v>
       </c>

</xml_diff>

<commit_message>
converter to app specific values
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec_v4.xlsx
+++ b/1-SystemDocs/System_spec_v4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="12960" windowHeight="11760" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="12960" windowHeight="11760" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -3403,21 +3403,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3441,6 +3426,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3907,11 +3907,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385728952"/>
-        <c:axId val="385730912"/>
+        <c:axId val="393190864"/>
+        <c:axId val="528020152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385728952"/>
+        <c:axId val="393190864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3956,12 +3956,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385730912"/>
+        <c:crossAx val="528020152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385730912"/>
+        <c:axId val="528020152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1400"/>
@@ -4020,7 +4020,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385728952"/>
+        <c:crossAx val="393190864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4736,7 +4736,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5679,7 +5679,7 @@
   <dimension ref="B1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8824,8 +8824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V63"/>
   <sheetViews>
-    <sheetView topLeftCell="B34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21:S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8852,19 +8852,19 @@
       </c>
     </row>
     <row r="3" spans="2:22" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="210" t="s">
+      <c r="B3" s="218" t="s">
         <v>537</v>
       </c>
-      <c r="C3" s="210"/>
-      <c r="D3" s="210"/>
-      <c r="E3" s="210"/>
-      <c r="F3" s="210"/>
-      <c r="G3" s="210"/>
-      <c r="H3" s="210"/>
-      <c r="I3" s="210"/>
-      <c r="J3" s="210"/>
-      <c r="K3" s="210"/>
-      <c r="L3" s="210"/>
+      <c r="C3" s="218"/>
+      <c r="D3" s="218"/>
+      <c r="E3" s="218"/>
+      <c r="F3" s="218"/>
+      <c r="G3" s="218"/>
+      <c r="H3" s="218"/>
+      <c r="I3" s="218"/>
+      <c r="J3" s="218"/>
+      <c r="K3" s="218"/>
+      <c r="L3" s="218"/>
       <c r="M3" s="129"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
@@ -9003,16 +9003,16 @@
       <c r="B10" s="151" t="s">
         <v>636</v>
       </c>
-      <c r="C10" s="211" t="s">
+      <c r="C10" s="219" t="s">
         <v>643</v>
       </c>
-      <c r="D10" s="211"/>
-      <c r="E10" s="211"/>
-      <c r="F10" s="211"/>
-      <c r="G10" s="211"/>
-      <c r="H10" s="211"/>
-      <c r="I10" s="211"/>
-      <c r="J10" s="212"/>
+      <c r="D10" s="219"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="219"/>
+      <c r="H10" s="219"/>
+      <c r="I10" s="219"/>
+      <c r="J10" s="220"/>
       <c r="T10" s="22">
         <v>9</v>
       </c>
@@ -9027,16 +9027,16 @@
       <c r="B11" s="151" t="s">
         <v>642</v>
       </c>
-      <c r="C11" s="211" t="s">
+      <c r="C11" s="219" t="s">
         <v>645</v>
       </c>
-      <c r="D11" s="211"/>
-      <c r="E11" s="211"/>
-      <c r="F11" s="211"/>
-      <c r="G11" s="211"/>
-      <c r="H11" s="211"/>
-      <c r="I11" s="211"/>
-      <c r="J11" s="212"/>
+      <c r="D11" s="219"/>
+      <c r="E11" s="219"/>
+      <c r="F11" s="219"/>
+      <c r="G11" s="219"/>
+      <c r="H11" s="219"/>
+      <c r="I11" s="219"/>
+      <c r="J11" s="220"/>
       <c r="T11" s="24" t="s">
         <v>102</v>
       </c>
@@ -9051,16 +9051,16 @@
       <c r="B12" s="144" t="s">
         <v>641</v>
       </c>
-      <c r="C12" s="213" t="s">
+      <c r="C12" s="221" t="s">
         <v>644</v>
       </c>
-      <c r="D12" s="213"/>
-      <c r="E12" s="213"/>
-      <c r="F12" s="213"/>
-      <c r="G12" s="213"/>
-      <c r="H12" s="213"/>
-      <c r="I12" s="213"/>
-      <c r="J12" s="214"/>
+      <c r="D12" s="221"/>
+      <c r="E12" s="221"/>
+      <c r="F12" s="221"/>
+      <c r="G12" s="221"/>
+      <c r="H12" s="221"/>
+      <c r="I12" s="221"/>
+      <c r="J12" s="222"/>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -9073,26 +9073,26 @@
       </c>
       <c r="C15" s="159"/>
       <c r="D15" s="159"/>
-      <c r="E15" s="219" t="s">
+      <c r="E15" s="214" t="s">
         <v>681</v>
       </c>
-      <c r="F15" s="220"/>
-      <c r="G15" s="221"/>
+      <c r="F15" s="215"/>
+      <c r="G15" s="216"/>
       <c r="H15" s="159"/>
       <c r="I15" s="159"/>
       <c r="J15" s="160"/>
-      <c r="L15" s="222" t="s">
+      <c r="L15" s="217" t="s">
         <v>706</v>
       </c>
-      <c r="M15" s="222"/>
-      <c r="N15" s="222"/>
-      <c r="O15" s="222"/>
-      <c r="P15" s="222"/>
-      <c r="Q15" s="222"/>
-      <c r="R15" s="222"/>
+      <c r="M15" s="217"/>
+      <c r="N15" s="217"/>
+      <c r="O15" s="217"/>
+      <c r="P15" s="217"/>
+      <c r="Q15" s="217"/>
+      <c r="R15" s="217"/>
     </row>
     <row r="16" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="215">
+      <c r="B16" s="210">
         <v>1</v>
       </c>
       <c r="C16" s="28" t="s">
@@ -9143,13 +9143,13 @@
       <c r="S16" s="182" t="s">
         <v>758</v>
       </c>
-      <c r="U16" s="218" t="s">
+      <c r="U16" s="213" t="s">
         <v>659</v>
       </c>
-      <c r="V16" s="218"/>
+      <c r="V16" s="213"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="216"/>
+      <c r="B17" s="211"/>
       <c r="C17" s="31" t="s">
         <v>428</v>
       </c>
@@ -9211,7 +9211,7 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="216"/>
+      <c r="B18" s="211"/>
       <c r="C18" s="31" t="s">
         <v>433</v>
       </c>
@@ -9232,7 +9232,7 @@
       </c>
     </row>
     <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="217"/>
+      <c r="B19" s="212"/>
       <c r="C19" s="35" t="s">
         <v>648</v>
       </c>
@@ -9251,7 +9251,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="215">
+      <c r="B20" s="210">
         <v>2</v>
       </c>
       <c r="C20" s="28" t="s">
@@ -9286,7 +9286,7 @@
       </c>
     </row>
     <row r="21" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="216"/>
+      <c r="B21" s="211"/>
       <c r="C21" s="31" t="s">
         <v>424</v>
       </c>
@@ -9356,7 +9356,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="216"/>
+      <c r="B22" s="211"/>
       <c r="C22" s="31" t="s">
         <v>425</v>
       </c>
@@ -9426,7 +9426,7 @@
       </c>
     </row>
     <row r="23" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="216"/>
+      <c r="B23" s="211"/>
       <c r="C23" s="31" t="s">
         <v>426</v>
       </c>
@@ -9496,7 +9496,7 @@
       </c>
     </row>
     <row r="24" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="216"/>
+      <c r="B24" s="211"/>
       <c r="C24" s="81" t="s">
         <v>427</v>
       </c>
@@ -9566,7 +9566,7 @@
       </c>
     </row>
     <row r="25" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="216"/>
+      <c r="B25" s="211"/>
       <c r="C25" s="31" t="s">
         <v>428</v>
       </c>
@@ -9636,7 +9636,7 @@
       </c>
     </row>
     <row r="26" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="216"/>
+      <c r="B26" s="211"/>
       <c r="C26" s="31" t="s">
         <v>429</v>
       </c>
@@ -9703,7 +9703,7 @@
       </c>
     </row>
     <row r="27" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="216"/>
+      <c r="B27" s="211"/>
       <c r="C27" s="81" t="s">
         <v>430</v>
       </c>
@@ -9770,7 +9770,7 @@
       </c>
     </row>
     <row r="28" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="216"/>
+      <c r="B28" s="211"/>
       <c r="C28" s="31" t="s">
         <v>431</v>
       </c>
@@ -9799,7 +9799,7 @@
       </c>
     </row>
     <row r="29" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="216"/>
+      <c r="B29" s="211"/>
       <c r="C29" s="31" t="s">
         <v>433</v>
       </c>
@@ -9828,7 +9828,7 @@
       </c>
     </row>
     <row r="30" spans="2:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="217"/>
+      <c r="B30" s="212"/>
       <c r="C30" s="35" t="s">
         <v>434</v>
       </c>
@@ -9857,7 +9857,7 @@
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="215">
+      <c r="B31" s="210">
         <v>3</v>
       </c>
       <c r="C31" s="28" t="s">
@@ -9897,7 +9897,7 @@
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B32" s="216"/>
+      <c r="B32" s="211"/>
       <c r="C32" s="31" t="s">
         <v>424</v>
       </c>
@@ -9941,7 +9941,7 @@
       </c>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B33" s="216"/>
+      <c r="B33" s="211"/>
       <c r="C33" s="31" t="s">
         <v>425</v>
       </c>
@@ -9985,7 +9985,7 @@
       </c>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B34" s="216"/>
+      <c r="B34" s="211"/>
       <c r="C34" s="31" t="s">
         <v>426</v>
       </c>
@@ -10026,7 +10026,7 @@
       </c>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B35" s="216"/>
+      <c r="B35" s="211"/>
       <c r="C35" s="81" t="s">
         <v>427</v>
       </c>
@@ -10070,7 +10070,7 @@
       </c>
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B36" s="216"/>
+      <c r="B36" s="211"/>
       <c r="C36" s="31" t="s">
         <v>428</v>
       </c>
@@ -10114,7 +10114,7 @@
       </c>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="216"/>
+      <c r="B37" s="211"/>
       <c r="C37" s="31" t="s">
         <v>429</v>
       </c>
@@ -10158,7 +10158,7 @@
       </c>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B38" s="216"/>
+      <c r="B38" s="211"/>
       <c r="C38" s="81" t="s">
         <v>430</v>
       </c>
@@ -10189,7 +10189,7 @@
       </c>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B39" s="216"/>
+      <c r="B39" s="211"/>
       <c r="C39" s="31" t="s">
         <v>431</v>
       </c>
@@ -10217,7 +10217,7 @@
       </c>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B40" s="216"/>
+      <c r="B40" s="211"/>
       <c r="C40" s="31" t="s">
         <v>433</v>
       </c>
@@ -10246,7 +10246,7 @@
       </c>
     </row>
     <row r="41" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="217"/>
+      <c r="B41" s="212"/>
       <c r="C41" s="35" t="s">
         <v>434</v>
       </c>
@@ -10277,7 +10277,7 @@
       </c>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B42" s="215">
+      <c r="B42" s="210">
         <v>4</v>
       </c>
       <c r="C42" s="28" t="s">
@@ -10317,7 +10317,7 @@
       </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B43" s="216"/>
+      <c r="B43" s="211"/>
       <c r="C43" s="31" t="s">
         <v>424</v>
       </c>
@@ -10361,7 +10361,7 @@
       </c>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B44" s="216"/>
+      <c r="B44" s="211"/>
       <c r="C44" s="31" t="s">
         <v>425</v>
       </c>
@@ -10405,7 +10405,7 @@
       </c>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B45" s="216"/>
+      <c r="B45" s="211"/>
       <c r="C45" s="31" t="s">
         <v>426</v>
       </c>
@@ -10436,7 +10436,7 @@
       </c>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B46" s="216"/>
+      <c r="B46" s="211"/>
       <c r="C46" s="81" t="s">
         <v>427</v>
       </c>
@@ -10467,7 +10467,7 @@
       </c>
     </row>
     <row r="47" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B47" s="216"/>
+      <c r="B47" s="211"/>
       <c r="C47" s="31" t="s">
         <v>428</v>
       </c>
@@ -10498,7 +10498,7 @@
       </c>
     </row>
     <row r="48" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B48" s="216"/>
+      <c r="B48" s="211"/>
       <c r="C48" s="31" t="s">
         <v>429</v>
       </c>
@@ -10529,7 +10529,7 @@
       </c>
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B49" s="216"/>
+      <c r="B49" s="211"/>
       <c r="C49" s="81" t="s">
         <v>430</v>
       </c>
@@ -10560,7 +10560,7 @@
       </c>
     </row>
     <row r="50" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B50" s="216"/>
+      <c r="B50" s="211"/>
       <c r="C50" s="31" t="s">
         <v>431</v>
       </c>
@@ -10591,7 +10591,7 @@
       </c>
     </row>
     <row r="51" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B51" s="216"/>
+      <c r="B51" s="211"/>
       <c r="C51" s="31" t="s">
         <v>433</v>
       </c>
@@ -10620,7 +10620,7 @@
       </c>
     </row>
     <row r="52" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="217"/>
+      <c r="B52" s="212"/>
       <c r="C52" s="35" t="s">
         <v>434</v>
       </c>
@@ -10651,7 +10651,7 @@
       </c>
     </row>
     <row r="53" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B53" s="215">
+      <c r="B53" s="210">
         <v>5</v>
       </c>
       <c r="C53" s="28" t="s">
@@ -10694,7 +10694,7 @@
       </c>
     </row>
     <row r="54" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B54" s="216"/>
+      <c r="B54" s="211"/>
       <c r="C54" s="31" t="s">
         <v>424</v>
       </c>
@@ -10738,7 +10738,7 @@
       </c>
     </row>
     <row r="55" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B55" s="216"/>
+      <c r="B55" s="211"/>
       <c r="C55" s="31" t="s">
         <v>425</v>
       </c>
@@ -10782,7 +10782,7 @@
       </c>
     </row>
     <row r="56" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B56" s="216"/>
+      <c r="B56" s="211"/>
       <c r="C56" s="31" t="s">
         <v>426</v>
       </c>
@@ -10826,7 +10826,7 @@
       </c>
     </row>
     <row r="57" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B57" s="216"/>
+      <c r="B57" s="211"/>
       <c r="C57" s="81" t="s">
         <v>427</v>
       </c>
@@ -10867,7 +10867,7 @@
       </c>
     </row>
     <row r="58" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B58" s="216"/>
+      <c r="B58" s="211"/>
       <c r="C58" s="31" t="s">
         <v>428</v>
       </c>
@@ -10898,7 +10898,7 @@
       </c>
     </row>
     <row r="59" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B59" s="216"/>
+      <c r="B59" s="211"/>
       <c r="C59" s="31" t="s">
         <v>429</v>
       </c>
@@ -10929,7 +10929,7 @@
       </c>
     </row>
     <row r="60" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B60" s="216"/>
+      <c r="B60" s="211"/>
       <c r="C60" s="81" t="s">
         <v>430</v>
       </c>
@@ -10952,7 +10952,7 @@
       </c>
     </row>
     <row r="61" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B61" s="216"/>
+      <c r="B61" s="211"/>
       <c r="C61" s="31" t="s">
         <v>431</v>
       </c>
@@ -10975,7 +10975,7 @@
       </c>
     </row>
     <row r="62" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B62" s="216"/>
+      <c r="B62" s="211"/>
       <c r="C62" s="31" t="s">
         <v>433</v>
       </c>
@@ -10996,7 +10996,7 @@
       </c>
     </row>
     <row r="63" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="217"/>
+      <c r="B63" s="212"/>
       <c r="C63" s="35" t="s">
         <v>434</v>
       </c>
@@ -11020,6 +11020,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C11:J11"/>
+    <mergeCell ref="C12:J12"/>
+    <mergeCell ref="B16:B19"/>
     <mergeCell ref="B31:B41"/>
     <mergeCell ref="B42:B52"/>
     <mergeCell ref="B53:B63"/>
@@ -11027,11 +11032,6 @@
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="L15:R15"/>
     <mergeCell ref="B20:B30"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="C11:J11"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="B16:B19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Contents!A1" display="Contents!A1"/>
@@ -12098,8 +12098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
V1.4 update conf set
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec_v4.xlsx
+++ b/1-SystemDocs/System_spec_v4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="12960" windowHeight="11760" firstSheet="10" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="12960" windowHeight="11760" tabRatio="760" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1809" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="781">
   <si>
     <t>ETH*</t>
   </si>
@@ -2432,6 +2432,15 @@
   </si>
   <si>
     <t>Others&gt;</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>H2</t>
   </si>
 </sst>
 </file>
@@ -3908,11 +3917,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385340288"/>
-        <c:axId val="385340680"/>
+        <c:axId val="204874312"/>
+        <c:axId val="204875096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385340288"/>
+        <c:axId val="204874312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3957,12 +3966,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385340680"/>
+        <c:crossAx val="204875096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385340680"/>
+        <c:axId val="204875096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1400"/>
@@ -4021,7 +4030,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385340288"/>
+        <c:crossAx val="204874312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5681,7 +5690,7 @@
   <dimension ref="B1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8824,10 +8833,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V63"/>
+  <dimension ref="B1:V74"/>
   <sheetViews>
-    <sheetView topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21:S26"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11020,8 +11029,270 @@
         <v>705</v>
       </c>
     </row>
+    <row r="64" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B64" s="215">
+        <v>6</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="D64" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="E64" s="164" t="s">
+        <v>560</v>
+      </c>
+      <c r="F64" s="164" t="s">
+        <v>561</v>
+      </c>
+      <c r="G64" s="164" t="s">
+        <v>562</v>
+      </c>
+      <c r="H64" s="155" t="s">
+        <v>560</v>
+      </c>
+      <c r="I64" s="155" t="s">
+        <v>561</v>
+      </c>
+      <c r="J64" s="156" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" s="216"/>
+      <c r="C65" s="31" t="s">
+        <v>424</v>
+      </c>
+      <c r="D65" s="31" t="s">
+        <v>651</v>
+      </c>
+      <c r="E65" s="166" t="s">
+        <v>708</v>
+      </c>
+      <c r="F65" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G65" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H65" s="157" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(E65,LEN(E65)-2),2))</f>
+        <v>0x18</v>
+      </c>
+      <c r="I65" s="157" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(F65,LEN(F65)-2),2))</f>
+        <v>0x00</v>
+      </c>
+      <c r="J65" s="158" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(G65,LEN(G65)-2),2))</f>
+        <v>0x03</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66" s="216"/>
+      <c r="C66" s="31" t="s">
+        <v>425</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E66" s="166" t="s">
+        <v>735</v>
+      </c>
+      <c r="F66" s="166" t="s">
+        <v>564</v>
+      </c>
+      <c r="G66" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H66" s="157" t="str">
+        <f t="shared" ref="H66" si="25">CONCATENATE("0x",BIN2HEX(RIGHT(E66,LEN(E66)-2),2))</f>
+        <v>0x0E</v>
+      </c>
+      <c r="I66" s="157" t="str">
+        <f t="shared" ref="I66" si="26">CONCATENATE("0x",BIN2HEX(RIGHT(F66,LEN(F66)-2),2))</f>
+        <v>0x40</v>
+      </c>
+      <c r="J66" s="158" t="str">
+        <f t="shared" ref="J66" si="27">CONCATENATE("0x",BIN2HEX(RIGHT(G66,LEN(G66)-2),2))</f>
+        <v>0x03</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67" s="216"/>
+      <c r="C67" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="D67" s="31" t="s">
+        <v>651</v>
+      </c>
+      <c r="E67" s="166" t="s">
+        <v>708</v>
+      </c>
+      <c r="F67" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G67" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H67" s="157" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(E67,LEN(E67)-2),2))</f>
+        <v>0x18</v>
+      </c>
+      <c r="I67" s="157" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(F67,LEN(F67)-2),2))</f>
+        <v>0x00</v>
+      </c>
+      <c r="J67" s="158" t="str">
+        <f>CONCATENATE("0x",BIN2HEX(RIGHT(G67,LEN(G67)-2),2))</f>
+        <v>0x03</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B68" s="216"/>
+      <c r="C68" s="81" t="s">
+        <v>427</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E68" s="166" t="s">
+        <v>735</v>
+      </c>
+      <c r="F68" s="166" t="s">
+        <v>564</v>
+      </c>
+      <c r="G68" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H68" s="157" t="str">
+        <f t="shared" ref="H68" si="28">CONCATENATE("0x",BIN2HEX(RIGHT(E68,LEN(E68)-2),2))</f>
+        <v>0x0E</v>
+      </c>
+      <c r="I68" s="157" t="str">
+        <f t="shared" ref="I68" si="29">CONCATENATE("0x",BIN2HEX(RIGHT(F68,LEN(F68)-2),2))</f>
+        <v>0x40</v>
+      </c>
+      <c r="J68" s="158" t="str">
+        <f t="shared" ref="J68" si="30">CONCATENATE("0x",BIN2HEX(RIGHT(G68,LEN(G68)-2),2))</f>
+        <v>0x03</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69" s="216"/>
+      <c r="C69" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="D69" s="87" t="s">
+        <v>780</v>
+      </c>
+      <c r="E69" s="166" t="s">
+        <v>710</v>
+      </c>
+      <c r="F69" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G69" s="165" t="s">
+        <v>583</v>
+      </c>
+      <c r="H69" s="157" t="s">
+        <v>600</v>
+      </c>
+      <c r="I69" s="157" t="s">
+        <v>778</v>
+      </c>
+      <c r="J69" s="158" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70" s="216"/>
+      <c r="C70" s="31" t="s">
+        <v>429</v>
+      </c>
+      <c r="D70" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H70" s="157"/>
+      <c r="I70" s="157"/>
+      <c r="J70" s="158"/>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B71" s="216"/>
+      <c r="C71" s="81" t="s">
+        <v>430</v>
+      </c>
+      <c r="D71" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H71" s="157"/>
+      <c r="I71" s="157"/>
+      <c r="J71" s="158"/>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B72" s="216"/>
+      <c r="C72" s="31" t="s">
+        <v>431</v>
+      </c>
+      <c r="D72" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E72" s="137"/>
+      <c r="F72" s="137"/>
+      <c r="G72" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H72" s="157"/>
+      <c r="I72" s="157"/>
+      <c r="J72" s="158"/>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B73" s="216"/>
+      <c r="C73" s="31" t="s">
+        <v>433</v>
+      </c>
+      <c r="D73" s="87" t="s">
+        <v>759</v>
+      </c>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="165" t="s">
+        <v>563</v>
+      </c>
+      <c r="H73" s="157"/>
+      <c r="I73" s="157"/>
+      <c r="J73" s="158"/>
+    </row>
+    <row r="74" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="217"/>
+      <c r="C74" s="35" t="s">
+        <v>434</v>
+      </c>
+      <c r="D74" s="35" t="s">
+        <v>759</v>
+      </c>
+      <c r="E74" s="193"/>
+      <c r="F74" s="193"/>
+      <c r="G74" s="194" t="s">
+        <v>563</v>
+      </c>
+      <c r="H74" s="162"/>
+      <c r="I74" s="162"/>
+      <c r="J74" s="163"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="B64:B74"/>
     <mergeCell ref="B31:B41"/>
     <mergeCell ref="B42:B52"/>
     <mergeCell ref="B53:B63"/>
@@ -11049,7 +11320,7 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12710,8 +12981,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bug fix app spec converter
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec_v4.xlsx
+++ b/1-SystemDocs/System_spec_v4.xlsx
@@ -3412,18 +3412,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3435,6 +3423,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3450,6 +3447,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3509,7 +3509,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3917,11 +3916,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="376538512"/>
-        <c:axId val="376538904"/>
+        <c:axId val="365119080"/>
+        <c:axId val="365117904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="376538512"/>
+        <c:axId val="365119080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3966,12 +3965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376538904"/>
+        <c:crossAx val="365117904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="376538904"/>
+        <c:axId val="365117904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1400"/>
@@ -4030,7 +4029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="376538512"/>
+        <c:crossAx val="365119080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4044,7 +4043,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4747,7 +4745,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8835,8 +8833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L74" sqref="L74"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8863,19 +8861,19 @@
       </c>
     </row>
     <row r="3" spans="2:22" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="218" t="s">
+      <c r="B3" s="217" t="s">
         <v>537</v>
       </c>
-      <c r="C3" s="218"/>
-      <c r="D3" s="218"/>
-      <c r="E3" s="218"/>
-      <c r="F3" s="218"/>
-      <c r="G3" s="218"/>
-      <c r="H3" s="218"/>
-      <c r="I3" s="218"/>
-      <c r="J3" s="218"/>
-      <c r="K3" s="218"/>
-      <c r="L3" s="218"/>
+      <c r="C3" s="217"/>
+      <c r="D3" s="217"/>
+      <c r="E3" s="217"/>
+      <c r="F3" s="217"/>
+      <c r="G3" s="217"/>
+      <c r="H3" s="217"/>
+      <c r="I3" s="217"/>
+      <c r="J3" s="217"/>
+      <c r="K3" s="217"/>
+      <c r="L3" s="217"/>
       <c r="M3" s="129"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
@@ -9014,16 +9012,16 @@
       <c r="B10" s="151" t="s">
         <v>636</v>
       </c>
-      <c r="C10" s="219" t="s">
+      <c r="C10" s="218" t="s">
         <v>643</v>
       </c>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="219"/>
-      <c r="H10" s="219"/>
-      <c r="I10" s="219"/>
-      <c r="J10" s="220"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
+      <c r="F10" s="218"/>
+      <c r="G10" s="218"/>
+      <c r="H10" s="218"/>
+      <c r="I10" s="218"/>
+      <c r="J10" s="219"/>
       <c r="T10" s="22">
         <v>9</v>
       </c>
@@ -9038,16 +9036,16 @@
       <c r="B11" s="151" t="s">
         <v>642</v>
       </c>
-      <c r="C11" s="219" t="s">
+      <c r="C11" s="218" t="s">
         <v>645</v>
       </c>
-      <c r="D11" s="219"/>
-      <c r="E11" s="219"/>
-      <c r="F11" s="219"/>
-      <c r="G11" s="219"/>
-      <c r="H11" s="219"/>
-      <c r="I11" s="219"/>
-      <c r="J11" s="220"/>
+      <c r="D11" s="218"/>
+      <c r="E11" s="218"/>
+      <c r="F11" s="218"/>
+      <c r="G11" s="218"/>
+      <c r="H11" s="218"/>
+      <c r="I11" s="218"/>
+      <c r="J11" s="219"/>
       <c r="T11" s="24" t="s">
         <v>102</v>
       </c>
@@ -9062,16 +9060,16 @@
       <c r="B12" s="144" t="s">
         <v>641</v>
       </c>
-      <c r="C12" s="221" t="s">
+      <c r="C12" s="220" t="s">
         <v>644</v>
       </c>
-      <c r="D12" s="221"/>
-      <c r="E12" s="221"/>
-      <c r="F12" s="221"/>
-      <c r="G12" s="221"/>
-      <c r="H12" s="221"/>
-      <c r="I12" s="221"/>
-      <c r="J12" s="222"/>
+      <c r="D12" s="220"/>
+      <c r="E12" s="220"/>
+      <c r="F12" s="220"/>
+      <c r="G12" s="220"/>
+      <c r="H12" s="220"/>
+      <c r="I12" s="220"/>
+      <c r="J12" s="221"/>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -9084,26 +9082,26 @@
       </c>
       <c r="C15" s="159"/>
       <c r="D15" s="159"/>
-      <c r="E15" s="214" t="s">
+      <c r="E15" s="210" t="s">
         <v>681</v>
       </c>
-      <c r="F15" s="215"/>
-      <c r="G15" s="216"/>
+      <c r="F15" s="211"/>
+      <c r="G15" s="212"/>
       <c r="H15" s="159"/>
       <c r="I15" s="159"/>
       <c r="J15" s="160"/>
-      <c r="L15" s="217" t="s">
+      <c r="L15" s="213" t="s">
         <v>706</v>
       </c>
-      <c r="M15" s="217"/>
-      <c r="N15" s="217"/>
-      <c r="O15" s="217"/>
-      <c r="P15" s="217"/>
-      <c r="Q15" s="217"/>
-      <c r="R15" s="217"/>
+      <c r="M15" s="213"/>
+      <c r="N15" s="213"/>
+      <c r="O15" s="213"/>
+      <c r="P15" s="213"/>
+      <c r="Q15" s="213"/>
+      <c r="R15" s="213"/>
     </row>
     <row r="16" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="210">
+      <c r="B16" s="214">
         <v>1</v>
       </c>
       <c r="C16" s="28" t="s">
@@ -9154,13 +9152,13 @@
       <c r="S16" s="182" t="s">
         <v>758</v>
       </c>
-      <c r="U16" s="213" t="s">
+      <c r="U16" s="222" t="s">
         <v>659</v>
       </c>
-      <c r="V16" s="213"/>
+      <c r="V16" s="222"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="211"/>
+      <c r="B17" s="215"/>
       <c r="C17" s="31" t="s">
         <v>428</v>
       </c>
@@ -9222,7 +9220,7 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="211"/>
+      <c r="B18" s="215"/>
       <c r="C18" s="31" t="s">
         <v>433</v>
       </c>
@@ -9243,7 +9241,7 @@
       </c>
     </row>
     <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="212"/>
+      <c r="B19" s="216"/>
       <c r="C19" s="35" t="s">
         <v>648</v>
       </c>
@@ -9262,7 +9260,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="210">
+      <c r="B20" s="214">
         <v>2</v>
       </c>
       <c r="C20" s="28" t="s">
@@ -9297,7 +9295,7 @@
       </c>
     </row>
     <row r="21" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="211"/>
+      <c r="B21" s="215"/>
       <c r="C21" s="31" t="s">
         <v>424</v>
       </c>
@@ -9367,7 +9365,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="211"/>
+      <c r="B22" s="215"/>
       <c r="C22" s="31" t="s">
         <v>425</v>
       </c>
@@ -9437,7 +9435,7 @@
       </c>
     </row>
     <row r="23" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="211"/>
+      <c r="B23" s="215"/>
       <c r="C23" s="31" t="s">
         <v>426</v>
       </c>
@@ -9507,7 +9505,7 @@
       </c>
     </row>
     <row r="24" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="211"/>
+      <c r="B24" s="215"/>
       <c r="C24" s="81" t="s">
         <v>427</v>
       </c>
@@ -9577,7 +9575,7 @@
       </c>
     </row>
     <row r="25" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="211"/>
+      <c r="B25" s="215"/>
       <c r="C25" s="31" t="s">
         <v>428</v>
       </c>
@@ -9647,7 +9645,7 @@
       </c>
     </row>
     <row r="26" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="211"/>
+      <c r="B26" s="215"/>
       <c r="C26" s="31" t="s">
         <v>429</v>
       </c>
@@ -9714,7 +9712,7 @@
       </c>
     </row>
     <row r="27" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="211"/>
+      <c r="B27" s="215"/>
       <c r="C27" s="81" t="s">
         <v>430</v>
       </c>
@@ -9781,7 +9779,7 @@
       </c>
     </row>
     <row r="28" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="211"/>
+      <c r="B28" s="215"/>
       <c r="C28" s="31" t="s">
         <v>431</v>
       </c>
@@ -9810,7 +9808,7 @@
       </c>
     </row>
     <row r="29" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="211"/>
+      <c r="B29" s="215"/>
       <c r="C29" s="31" t="s">
         <v>433</v>
       </c>
@@ -9839,7 +9837,7 @@
       </c>
     </row>
     <row r="30" spans="2:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="212"/>
+      <c r="B30" s="216"/>
       <c r="C30" s="35" t="s">
         <v>434</v>
       </c>
@@ -9868,7 +9866,7 @@
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="210">
+      <c r="B31" s="214">
         <v>3</v>
       </c>
       <c r="C31" s="28" t="s">
@@ -9908,7 +9906,7 @@
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B32" s="211"/>
+      <c r="B32" s="215"/>
       <c r="C32" s="31" t="s">
         <v>424</v>
       </c>
@@ -9952,7 +9950,7 @@
       </c>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B33" s="211"/>
+      <c r="B33" s="215"/>
       <c r="C33" s="31" t="s">
         <v>425</v>
       </c>
@@ -9996,7 +9994,7 @@
       </c>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B34" s="211"/>
+      <c r="B34" s="215"/>
       <c r="C34" s="31" t="s">
         <v>426</v>
       </c>
@@ -10037,7 +10035,7 @@
       </c>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B35" s="211"/>
+      <c r="B35" s="215"/>
       <c r="C35" s="81" t="s">
         <v>427</v>
       </c>
@@ -10081,7 +10079,7 @@
       </c>
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B36" s="211"/>
+      <c r="B36" s="215"/>
       <c r="C36" s="31" t="s">
         <v>428</v>
       </c>
@@ -10125,7 +10123,7 @@
       </c>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="211"/>
+      <c r="B37" s="215"/>
       <c r="C37" s="31" t="s">
         <v>429</v>
       </c>
@@ -10169,7 +10167,7 @@
       </c>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B38" s="211"/>
+      <c r="B38" s="215"/>
       <c r="C38" s="81" t="s">
         <v>430</v>
       </c>
@@ -10200,7 +10198,7 @@
       </c>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B39" s="211"/>
+      <c r="B39" s="215"/>
       <c r="C39" s="31" t="s">
         <v>431</v>
       </c>
@@ -10228,7 +10226,7 @@
       </c>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B40" s="211"/>
+      <c r="B40" s="215"/>
       <c r="C40" s="31" t="s">
         <v>433</v>
       </c>
@@ -10257,7 +10255,7 @@
       </c>
     </row>
     <row r="41" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="212"/>
+      <c r="B41" s="216"/>
       <c r="C41" s="35" t="s">
         <v>434</v>
       </c>
@@ -10288,7 +10286,7 @@
       </c>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B42" s="210">
+      <c r="B42" s="214">
         <v>4</v>
       </c>
       <c r="C42" s="28" t="s">
@@ -10328,7 +10326,7 @@
       </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B43" s="211"/>
+      <c r="B43" s="215"/>
       <c r="C43" s="31" t="s">
         <v>424</v>
       </c>
@@ -10372,7 +10370,7 @@
       </c>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B44" s="211"/>
+      <c r="B44" s="215"/>
       <c r="C44" s="31" t="s">
         <v>425</v>
       </c>
@@ -10416,7 +10414,7 @@
       </c>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B45" s="211"/>
+      <c r="B45" s="215"/>
       <c r="C45" s="31" t="s">
         <v>426</v>
       </c>
@@ -10447,7 +10445,7 @@
       </c>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B46" s="211"/>
+      <c r="B46" s="215"/>
       <c r="C46" s="81" t="s">
         <v>427</v>
       </c>
@@ -10478,7 +10476,7 @@
       </c>
     </row>
     <row r="47" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B47" s="211"/>
+      <c r="B47" s="215"/>
       <c r="C47" s="31" t="s">
         <v>428</v>
       </c>
@@ -10509,7 +10507,7 @@
       </c>
     </row>
     <row r="48" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B48" s="211"/>
+      <c r="B48" s="215"/>
       <c r="C48" s="31" t="s">
         <v>429</v>
       </c>
@@ -10540,7 +10538,7 @@
       </c>
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B49" s="211"/>
+      <c r="B49" s="215"/>
       <c r="C49" s="81" t="s">
         <v>430</v>
       </c>
@@ -10571,7 +10569,7 @@
       </c>
     </row>
     <row r="50" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B50" s="211"/>
+      <c r="B50" s="215"/>
       <c r="C50" s="31" t="s">
         <v>431</v>
       </c>
@@ -10602,7 +10600,7 @@
       </c>
     </row>
     <row r="51" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B51" s="211"/>
+      <c r="B51" s="215"/>
       <c r="C51" s="31" t="s">
         <v>433</v>
       </c>
@@ -10631,7 +10629,7 @@
       </c>
     </row>
     <row r="52" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="212"/>
+      <c r="B52" s="216"/>
       <c r="C52" s="35" t="s">
         <v>434</v>
       </c>
@@ -10662,7 +10660,7 @@
       </c>
     </row>
     <row r="53" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B53" s="210">
+      <c r="B53" s="214">
         <v>5</v>
       </c>
       <c r="C53" s="28" t="s">
@@ -10705,7 +10703,7 @@
       </c>
     </row>
     <row r="54" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B54" s="211"/>
+      <c r="B54" s="215"/>
       <c r="C54" s="31" t="s">
         <v>424</v>
       </c>
@@ -10749,7 +10747,7 @@
       </c>
     </row>
     <row r="55" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B55" s="211"/>
+      <c r="B55" s="215"/>
       <c r="C55" s="31" t="s">
         <v>425</v>
       </c>
@@ -10793,7 +10791,7 @@
       </c>
     </row>
     <row r="56" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B56" s="211"/>
+      <c r="B56" s="215"/>
       <c r="C56" s="31" t="s">
         <v>426</v>
       </c>
@@ -10837,7 +10835,7 @@
       </c>
     </row>
     <row r="57" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B57" s="211"/>
+      <c r="B57" s="215"/>
       <c r="C57" s="81" t="s">
         <v>427</v>
       </c>
@@ -10878,7 +10876,7 @@
       </c>
     </row>
     <row r="58" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B58" s="211"/>
+      <c r="B58" s="215"/>
       <c r="C58" s="31" t="s">
         <v>428</v>
       </c>
@@ -10909,7 +10907,7 @@
       </c>
     </row>
     <row r="59" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B59" s="211"/>
+      <c r="B59" s="215"/>
       <c r="C59" s="31" t="s">
         <v>429</v>
       </c>
@@ -10940,7 +10938,7 @@
       </c>
     </row>
     <row r="60" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B60" s="211"/>
+      <c r="B60" s="215"/>
       <c r="C60" s="81" t="s">
         <v>430</v>
       </c>
@@ -10963,7 +10961,7 @@
       </c>
     </row>
     <row r="61" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B61" s="211"/>
+      <c r="B61" s="215"/>
       <c r="C61" s="31" t="s">
         <v>431</v>
       </c>
@@ -10986,7 +10984,7 @@
       </c>
     </row>
     <row r="62" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B62" s="211"/>
+      <c r="B62" s="215"/>
       <c r="C62" s="31" t="s">
         <v>433</v>
       </c>
@@ -11007,7 +11005,7 @@
       </c>
     </row>
     <row r="63" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="212"/>
+      <c r="B63" s="216"/>
       <c r="C63" s="35" t="s">
         <v>434</v>
       </c>
@@ -11030,7 +11028,7 @@
       </c>
     </row>
     <row r="64" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B64" s="210">
+      <c r="B64" s="214">
         <v>6</v>
       </c>
       <c r="C64" s="28" t="s">
@@ -11059,7 +11057,7 @@
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="211"/>
+      <c r="B65" s="215"/>
       <c r="C65" s="31" t="s">
         <v>424</v>
       </c>
@@ -11089,7 +11087,7 @@
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="211"/>
+      <c r="B66" s="215"/>
       <c r="C66" s="31" t="s">
         <v>425</v>
       </c>
@@ -11119,7 +11117,7 @@
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="211"/>
+      <c r="B67" s="215"/>
       <c r="C67" s="31" t="s">
         <v>426</v>
       </c>
@@ -11149,7 +11147,7 @@
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="211"/>
+      <c r="B68" s="215"/>
       <c r="C68" s="81" t="s">
         <v>427</v>
       </c>
@@ -11179,7 +11177,7 @@
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" s="211"/>
+      <c r="B69" s="215"/>
       <c r="C69" s="31" t="s">
         <v>428</v>
       </c>
@@ -11206,7 +11204,7 @@
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" s="211"/>
+      <c r="B70" s="215"/>
       <c r="C70" s="31" t="s">
         <v>429</v>
       </c>
@@ -11223,7 +11221,7 @@
       <c r="J70" s="158"/>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" s="211"/>
+      <c r="B71" s="215"/>
       <c r="C71" s="81" t="s">
         <v>430</v>
       </c>
@@ -11240,7 +11238,7 @@
       <c r="J71" s="158"/>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" s="211"/>
+      <c r="B72" s="215"/>
       <c r="C72" s="31" t="s">
         <v>431</v>
       </c>
@@ -11257,7 +11255,7 @@
       <c r="J72" s="158"/>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" s="211"/>
+      <c r="B73" s="215"/>
       <c r="C73" s="31" t="s">
         <v>433</v>
       </c>
@@ -11274,7 +11272,7 @@
       <c r="J73" s="158"/>
     </row>
     <row r="74" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="212"/>
+      <c r="B74" s="216"/>
       <c r="C74" s="35" t="s">
         <v>434</v>
       </c>
@@ -11292,6 +11290,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B64:B74"/>
+    <mergeCell ref="B31:B41"/>
+    <mergeCell ref="B42:B52"/>
+    <mergeCell ref="B53:B63"/>
+    <mergeCell ref="U16:V16"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="L15:R15"/>
     <mergeCell ref="B20:B30"/>
@@ -11300,11 +11303,6 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B64:B74"/>
-    <mergeCell ref="B31:B41"/>
-    <mergeCell ref="B42:B52"/>
-    <mergeCell ref="B53:B63"/>
-    <mergeCell ref="U16:V16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Contents!A1" display="Contents!A1"/>

</xml_diff>

<commit_message>
button stop measurement fcn, static fallback IP, V1.7 release
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec_v4.xlsx
+++ b/1-SystemDocs/System_spec_v4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="12960" windowHeight="11760" tabRatio="760" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="12960" windowHeight="11760" tabRatio="760" firstSheet="12" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="794">
   <si>
     <t>ETH*</t>
   </si>
@@ -1514,9 +1514,6 @@
     <t>Period [s]</t>
   </si>
   <si>
-    <t>Waiting for DHCP (max 60 seconds)</t>
-  </si>
-  <si>
     <t>Blinking</t>
   </si>
   <si>
@@ -1794,9 +1791,6 @@
   </si>
   <si>
     <t>Add sampling period to SD file or time</t>
-  </si>
-  <si>
-    <t>Button press registered, pressed 1 to 4s, measurement will start on button release</t>
   </si>
   <si>
     <t>Button press registered, pressed 4 - 15s, Unit will restart on release or after 15s from press</t>
@@ -2441,6 +2435,87 @@
   </si>
   <si>
     <t>H2</t>
+  </si>
+  <si>
+    <t>Button press registered, pressed 1 to 4s, measurement will start on button release, if measurement is currently active then it will stop</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Waiting for DHCP (max 60 seconds). If button is pressed for 1s in this period - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fallback IP settings are used</t>
+    </r>
+  </si>
+  <si>
+    <t>fallback IP settings</t>
+  </si>
+  <si>
+    <t>Device IP</t>
+  </si>
+  <si>
+    <t>Device gateway</t>
+  </si>
+  <si>
+    <t>Device mask:</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>For direct connection</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Gateway</t>
+  </si>
+  <si>
+    <t>Mask:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Interconnect with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>crossed ETH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cable</t>
+    </r>
+  </si>
+  <si>
+    <t>configure computer to</t>
+  </si>
+  <si>
+    <t>192.168.5.200</t>
+  </si>
+  <si>
+    <t>192.168.5.1</t>
   </si>
 </sst>
 </file>
@@ -3027,7 +3102,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="232">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3449,6 +3524,33 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3916,11 +4018,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="365119080"/>
-        <c:axId val="365117904"/>
+        <c:axId val="393241104"/>
+        <c:axId val="393241496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="365119080"/>
+        <c:axId val="393241104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3965,12 +4067,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365117904"/>
+        <c:crossAx val="393241496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="365117904"/>
+        <c:axId val="393241496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1400"/>
@@ -4029,7 +4131,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="365119080"/>
+        <c:crossAx val="393241104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5688,7 +5790,7 @@
   <dimension ref="B1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5748,13 +5850,13 @@
     </row>
     <row r="11" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B11" s="55" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C11" s="15"/>
     </row>
     <row r="12" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B12" s="55" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C12" s="15"/>
     </row>
@@ -5895,7 +5997,7 @@
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="M2" s="76"/>
     </row>
@@ -5904,13 +6006,13 @@
         <v>402</v>
       </c>
       <c r="D3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I3" s="136" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="L3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="M3" s="76"/>
     </row>
@@ -5925,7 +6027,7 @@
         <v>404</v>
       </c>
       <c r="E4" s="108" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F4" s="108" t="s">
         <v>405</v>
@@ -5937,7 +6039,7 @@
         <v>243</v>
       </c>
       <c r="I4" s="133" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="L4" s="105" t="s">
         <v>422</v>
@@ -5968,7 +6070,7 @@
       </c>
       <c r="H5" s="67"/>
       <c r="I5" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L5" s="101">
         <v>6</v>
@@ -5999,7 +6101,7 @@
       </c>
       <c r="H6" s="67"/>
       <c r="I6" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L6" s="101">
         <f>L5+3</f>
@@ -6031,7 +6133,7 @@
       </c>
       <c r="H7" s="67"/>
       <c r="I7" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L7" s="101">
         <f t="shared" ref="L7:L16" si="1">L6+3</f>
@@ -6063,7 +6165,7 @@
       </c>
       <c r="H8" s="67"/>
       <c r="I8" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L8" s="101">
         <f t="shared" si="1"/>
@@ -6095,7 +6197,7 @@
       </c>
       <c r="H9" s="67"/>
       <c r="I9" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L9" s="101">
         <f t="shared" si="1"/>
@@ -6127,7 +6229,7 @@
       </c>
       <c r="H10" s="67"/>
       <c r="I10" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L10" s="101">
         <f t="shared" si="1"/>
@@ -6159,7 +6261,7 @@
       </c>
       <c r="H11" s="67"/>
       <c r="I11" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L11" s="101">
         <f t="shared" si="1"/>
@@ -6191,7 +6293,7 @@
       </c>
       <c r="H12" s="69"/>
       <c r="I12" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L12" s="101">
         <f t="shared" si="1"/>
@@ -6223,7 +6325,7 @@
       </c>
       <c r="H13" s="29"/>
       <c r="I13" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L13" s="101">
         <f t="shared" si="1"/>
@@ -6255,7 +6357,7 @@
       </c>
       <c r="H14" s="32"/>
       <c r="I14" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L14" s="101">
         <f t="shared" si="1"/>
@@ -6287,7 +6389,7 @@
       </c>
       <c r="H15" s="32"/>
       <c r="I15" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L15" s="101">
         <f t="shared" si="1"/>
@@ -6319,7 +6421,7 @@
       </c>
       <c r="H16" s="32"/>
       <c r="I16" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L16" s="103">
         <f t="shared" si="1"/>
@@ -6351,7 +6453,7 @@
       </c>
       <c r="H17" s="32"/>
       <c r="I17" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="M17" s="76"/>
     </row>
@@ -6377,7 +6479,7 @@
       </c>
       <c r="H18" s="32"/>
       <c r="I18" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="M18" s="76"/>
     </row>
@@ -6403,7 +6505,7 @@
       </c>
       <c r="H19" s="32"/>
       <c r="I19" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L19" s="87"/>
     </row>
@@ -6429,13 +6531,13 @@
       </c>
       <c r="H20" s="36"/>
       <c r="I20" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L20" s="113" t="s">
+        <v>494</v>
+      </c>
+      <c r="M20" s="29" t="s">
         <v>495</v>
-      </c>
-      <c r="M20" s="29" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
@@ -6460,7 +6562,7 @@
       </c>
       <c r="H21" s="29"/>
       <c r="I21" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L21" s="30">
         <v>28000</v>
@@ -6492,10 +6594,10 @@
       </c>
       <c r="H22" s="32"/>
       <c r="I22" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L22" s="114" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="M22" s="32"/>
     </row>
@@ -6521,7 +6623,7 @@
       </c>
       <c r="H23" s="32"/>
       <c r="I23" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L23" s="34">
         <v>23000</v>
@@ -6553,7 +6655,7 @@
       </c>
       <c r="H24" s="32"/>
       <c r="I24" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L24" s="76"/>
     </row>
@@ -6579,7 +6681,7 @@
       </c>
       <c r="H25" s="32"/>
       <c r="I25" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L25" s="76"/>
     </row>
@@ -6605,7 +6707,7 @@
       </c>
       <c r="H26" s="32"/>
       <c r="I26" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="L26" s="76"/>
     </row>
@@ -6631,7 +6733,7 @@
       </c>
       <c r="H27" s="32"/>
       <c r="I27" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="28" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6656,7 +6758,7 @@
       </c>
       <c r="H28" s="36"/>
       <c r="I28" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
@@ -6681,7 +6783,7 @@
       </c>
       <c r="H29" s="29"/>
       <c r="I29" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J29" s="112"/>
       <c r="K29" s="112"/>
@@ -6708,7 +6810,7 @@
       </c>
       <c r="H30" s="32"/>
       <c r="I30" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J30" s="112"/>
       <c r="K30" s="112"/>
@@ -6735,7 +6837,7 @@
       </c>
       <c r="H31" s="32"/>
       <c r="I31" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J31" s="112"/>
       <c r="K31" s="112"/>
@@ -6762,7 +6864,7 @@
       </c>
       <c r="H32" s="32"/>
       <c r="I32" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
@@ -6787,7 +6889,7 @@
       </c>
       <c r="H33" s="32"/>
       <c r="I33" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -6812,7 +6914,7 @@
       </c>
       <c r="H34" s="32"/>
       <c r="I34" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -6837,7 +6939,7 @@
       </c>
       <c r="H35" s="32"/>
       <c r="I35" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6862,7 +6964,7 @@
       </c>
       <c r="H36" s="32"/>
       <c r="I36" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
@@ -6887,7 +6989,7 @@
       </c>
       <c r="H37" s="124"/>
       <c r="I37" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
@@ -6912,7 +7014,7 @@
       </c>
       <c r="H38" s="67"/>
       <c r="I38" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
@@ -6937,7 +7039,7 @@
       </c>
       <c r="H39" s="67"/>
       <c r="I39" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
@@ -6962,7 +7064,7 @@
       </c>
       <c r="H40" s="67"/>
       <c r="I40" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
@@ -6987,7 +7089,7 @@
       </c>
       <c r="H41" s="67"/>
       <c r="I41" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
@@ -7012,7 +7114,7 @@
       </c>
       <c r="H42" s="67"/>
       <c r="I42" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
@@ -7037,7 +7139,7 @@
       </c>
       <c r="H43" s="67"/>
       <c r="I43" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7062,7 +7164,7 @@
       </c>
       <c r="H44" s="69"/>
       <c r="I44" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
@@ -7087,7 +7189,7 @@
       </c>
       <c r="H45" s="32"/>
       <c r="I45" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
@@ -7112,7 +7214,7 @@
       </c>
       <c r="H46" s="32"/>
       <c r="I46" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
@@ -7137,7 +7239,7 @@
       </c>
       <c r="H47" s="32"/>
       <c r="I47" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
@@ -7162,7 +7264,7 @@
       </c>
       <c r="H48" s="32"/>
       <c r="I48" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
@@ -7187,7 +7289,7 @@
       </c>
       <c r="H49" s="32"/>
       <c r="I49" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
@@ -7212,7 +7314,7 @@
       </c>
       <c r="H50" s="32"/>
       <c r="I50" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
@@ -7237,7 +7339,7 @@
       </c>
       <c r="H51" s="32"/>
       <c r="I51" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="52" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7262,7 +7364,7 @@
       </c>
       <c r="H52" s="36"/>
       <c r="I52" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
@@ -7287,7 +7389,7 @@
       </c>
       <c r="H53" s="29"/>
       <c r="I53" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
@@ -7312,7 +7414,7 @@
       </c>
       <c r="H54" s="32"/>
       <c r="I54" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
@@ -7337,7 +7439,7 @@
       </c>
       <c r="H55" s="32"/>
       <c r="I55" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
@@ -7362,7 +7464,7 @@
       </c>
       <c r="H56" s="32"/>
       <c r="I56" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
@@ -7387,7 +7489,7 @@
       </c>
       <c r="H57" s="32"/>
       <c r="I57" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
@@ -7412,7 +7514,7 @@
       </c>
       <c r="H58" s="32"/>
       <c r="I58" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
@@ -7437,7 +7539,7 @@
       </c>
       <c r="H59" s="32"/>
       <c r="I59" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="60" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7462,7 +7564,7 @@
       </c>
       <c r="H60" s="36"/>
       <c r="I60" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
@@ -7487,7 +7589,7 @@
       </c>
       <c r="H61" s="29"/>
       <c r="I61" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
@@ -7512,7 +7614,7 @@
       </c>
       <c r="H62" s="32"/>
       <c r="I62" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
@@ -7537,7 +7639,7 @@
       </c>
       <c r="H63" s="32"/>
       <c r="I63" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
@@ -7562,7 +7664,7 @@
       </c>
       <c r="H64" s="32"/>
       <c r="I64" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
@@ -7587,7 +7689,7 @@
       </c>
       <c r="H65" s="32"/>
       <c r="I65" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
@@ -7612,7 +7714,7 @@
       </c>
       <c r="H66" s="32"/>
       <c r="I66" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
@@ -7637,7 +7739,7 @@
       </c>
       <c r="H67" s="32"/>
       <c r="I67" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="68" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7662,7 +7764,7 @@
       </c>
       <c r="H68" s="36"/>
       <c r="I68" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
@@ -7687,7 +7789,7 @@
       </c>
       <c r="H69" s="124"/>
       <c r="I69" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
@@ -7712,7 +7814,7 @@
       </c>
       <c r="H70" s="67"/>
       <c r="I70" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
@@ -7737,7 +7839,7 @@
       </c>
       <c r="H71" s="67"/>
       <c r="I71" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
@@ -7762,7 +7864,7 @@
       </c>
       <c r="H72" s="67"/>
       <c r="I72" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
@@ -7787,7 +7889,7 @@
       </c>
       <c r="H73" s="67"/>
       <c r="I73" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
@@ -7812,7 +7914,7 @@
       </c>
       <c r="H74" s="67"/>
       <c r="I74" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
@@ -7837,7 +7939,7 @@
       </c>
       <c r="H75" s="67"/>
       <c r="I75" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="76" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7862,7 +7964,7 @@
       </c>
       <c r="H76" s="69"/>
       <c r="I76" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
@@ -7887,7 +7989,7 @@
       </c>
       <c r="H77" s="32"/>
       <c r="I77" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
@@ -7912,7 +8014,7 @@
       </c>
       <c r="H78" s="32"/>
       <c r="I78" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
@@ -7937,7 +8039,7 @@
       </c>
       <c r="H79" s="32"/>
       <c r="I79" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
@@ -7962,7 +8064,7 @@
       </c>
       <c r="H80" s="32"/>
       <c r="I80" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
@@ -7987,7 +8089,7 @@
       </c>
       <c r="H81" s="32"/>
       <c r="I81" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
@@ -8012,7 +8114,7 @@
       </c>
       <c r="H82" s="32"/>
       <c r="I82" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
@@ -8037,7 +8139,7 @@
       </c>
       <c r="H83" s="32"/>
       <c r="I83" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="84" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8062,12 +8164,12 @@
       </c>
       <c r="H84" s="36"/>
       <c r="I84" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="118" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C85" s="119">
         <f t="shared" si="4"/>
@@ -8087,12 +8189,12 @@
       </c>
       <c r="H85" s="29"/>
       <c r="I85" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="115" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C86" s="10">
         <f t="shared" si="4"/>
@@ -8112,12 +8214,12 @@
       </c>
       <c r="H86" s="32"/>
       <c r="I86" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="115" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C87" s="10">
         <f t="shared" si="4"/>
@@ -8137,12 +8239,12 @@
       </c>
       <c r="H87" s="32"/>
       <c r="I87" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="115" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C88" s="10">
         <f t="shared" si="4"/>
@@ -8162,12 +8264,12 @@
       </c>
       <c r="H88" s="32"/>
       <c r="I88" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="115" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C89" s="10">
         <f t="shared" si="4"/>
@@ -8187,12 +8289,12 @@
       </c>
       <c r="H89" s="32"/>
       <c r="I89" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="115" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C90" s="10">
         <f t="shared" si="4"/>
@@ -8212,12 +8314,12 @@
       </c>
       <c r="H90" s="32"/>
       <c r="I90" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="115" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C91" s="10">
         <f t="shared" si="4"/>
@@ -8237,12 +8339,12 @@
       </c>
       <c r="H91" s="32"/>
       <c r="I91" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="92" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B92" s="121" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C92" s="122">
         <f t="shared" si="4"/>
@@ -8262,12 +8364,12 @@
       </c>
       <c r="H92" s="36"/>
       <c r="I92" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="118" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C93" s="119">
         <f t="shared" si="4"/>
@@ -8287,12 +8389,12 @@
       </c>
       <c r="H93" s="29"/>
       <c r="I93" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="115" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C94" s="10">
         <f t="shared" si="4"/>
@@ -8312,12 +8414,12 @@
       </c>
       <c r="H94" s="32"/>
       <c r="I94" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="115" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C95" s="10">
         <f t="shared" si="4"/>
@@ -8337,12 +8439,12 @@
       </c>
       <c r="H95" s="32"/>
       <c r="I95" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="115" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C96" s="10">
         <f t="shared" si="4"/>
@@ -8362,12 +8464,12 @@
       </c>
       <c r="H96" s="32"/>
       <c r="I96" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="115" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C97" s="10">
         <f t="shared" si="4"/>
@@ -8387,12 +8489,12 @@
       </c>
       <c r="H97" s="32"/>
       <c r="I97" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="115" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C98" s="10">
         <f t="shared" si="4"/>
@@ -8412,12 +8514,12 @@
       </c>
       <c r="H98" s="32"/>
       <c r="I98" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="115" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C99" s="10">
         <f t="shared" si="4"/>
@@ -8437,12 +8539,12 @@
       </c>
       <c r="H99" s="32"/>
       <c r="I99" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="100" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B100" s="121" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C100" s="122">
         <f t="shared" si="4"/>
@@ -8462,7 +8564,7 @@
       </c>
       <c r="H100" s="36"/>
       <c r="I100" s="134" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="101" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8485,158 +8587,158 @@
         <v>129</v>
       </c>
       <c r="H101" s="29" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I101" s="134"/>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="123" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C102" s="28">
         <f t="shared" ref="C102:C108" si="5">HEX2DEC(B102)</f>
         <v>240</v>
       </c>
       <c r="D102" s="125" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E102" s="125"/>
       <c r="F102" s="119" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G102" s="119" t="s">
+        <v>488</v>
+      </c>
+      <c r="H102" s="29" t="s">
         <v>489</v>
       </c>
-      <c r="H102" s="29" t="s">
-        <v>490</v>
-      </c>
       <c r="I102" s="135" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="110" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C103" s="31">
         <f t="shared" si="5"/>
         <v>241</v>
       </c>
       <c r="D103" s="87" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E103" s="87"/>
       <c r="F103" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="G103" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="H103" s="32" t="s">
         <v>489</v>
       </c>
-      <c r="H103" s="32" t="s">
-        <v>490</v>
-      </c>
       <c r="I103" s="135" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="110" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C104" s="31">
         <f t="shared" si="5"/>
         <v>242</v>
       </c>
       <c r="D104" s="87" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E104" s="87"/>
       <c r="F104" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G104" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="H104" s="32" t="s">
         <v>489</v>
       </c>
-      <c r="H104" s="32" t="s">
-        <v>490</v>
-      </c>
       <c r="I104" s="135" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="105" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="116" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C105" s="35">
         <f t="shared" si="5"/>
         <v>243</v>
       </c>
       <c r="D105" s="126" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E105" s="126"/>
       <c r="F105" s="122" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G105" s="122" t="s">
+        <v>488</v>
+      </c>
+      <c r="H105" s="36" t="s">
         <v>489</v>
       </c>
-      <c r="H105" s="36" t="s">
-        <v>490</v>
-      </c>
       <c r="I105" s="135" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="123" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C106" s="28">
         <f t="shared" si="5"/>
         <v>253</v>
       </c>
       <c r="D106" s="125" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E106" s="125"/>
       <c r="F106" s="119" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G106" s="119" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H106" s="29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I106" s="135" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="107" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B107" s="116" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C107" s="122">
         <f t="shared" si="5"/>
         <v>254</v>
       </c>
       <c r="D107" s="126" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E107" s="126"/>
       <c r="F107" s="122" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G107" s="122" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H107" s="36" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I107" s="135" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="108" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8693,16 +8795,16 @@
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="130" t="s">
+        <v>548</v>
+      </c>
+      <c r="C3" s="131" t="s">
         <v>549</v>
       </c>
-      <c r="C3" s="131" t="s">
+      <c r="D3" s="131" t="s">
         <v>550</v>
       </c>
-      <c r="D3" s="131" t="s">
+      <c r="E3" s="132" t="s">
         <v>551</v>
-      </c>
-      <c r="E3" s="132" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -8815,10 +8917,10 @@
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="D10" s="75" t="s">
+        <v>552</v>
+      </c>
+      <c r="E10" s="75" t="s">
         <v>553</v>
-      </c>
-      <c r="E10" s="75" t="s">
-        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -8833,7 +8935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
@@ -8862,7 +8964,7 @@
     </row>
     <row r="3" spans="2:22" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="217" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C3" s="217"/>
       <c r="D3" s="217"/>
@@ -8906,7 +9008,7 @@
     </row>
     <row r="6" spans="2:22" s="75" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="75" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P6" s="142"/>
       <c r="Q6" s="142"/>
@@ -8923,7 +9025,7 @@
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="145" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C7" s="146">
         <v>7</v>
@@ -8956,36 +9058,36 @@
         <v>283</v>
       </c>
       <c r="V7" s="127" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="148" t="s">
+        <v>633</v>
+      </c>
+      <c r="C8" s="149" t="s">
+        <v>639</v>
+      </c>
+      <c r="D8" s="149" t="s">
+        <v>639</v>
+      </c>
+      <c r="E8" s="149" t="s">
+        <v>639</v>
+      </c>
+      <c r="F8" s="149" t="s">
+        <v>638</v>
+      </c>
+      <c r="G8" s="149" t="s">
+        <v>637</v>
+      </c>
+      <c r="H8" s="149" t="s">
+        <v>636</v>
+      </c>
+      <c r="I8" s="149" t="s">
         <v>635</v>
       </c>
-      <c r="C8" s="149" t="s">
-        <v>641</v>
-      </c>
-      <c r="D8" s="149" t="s">
-        <v>641</v>
-      </c>
-      <c r="E8" s="149" t="s">
-        <v>641</v>
-      </c>
-      <c r="F8" s="149" t="s">
-        <v>640</v>
-      </c>
-      <c r="G8" s="149" t="s">
-        <v>639</v>
-      </c>
-      <c r="H8" s="149" t="s">
-        <v>638</v>
-      </c>
-      <c r="I8" s="149" t="s">
-        <v>637</v>
-      </c>
       <c r="J8" s="150" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="T8" s="22">
         <v>7</v>
@@ -8994,7 +9096,7 @@
         <v>283</v>
       </c>
       <c r="V8" s="23" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9005,15 +9107,15 @@
         <v>283</v>
       </c>
       <c r="V9" s="23" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="10" spans="2:22" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="151" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C10" s="218" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D10" s="218"/>
       <c r="E10" s="218"/>
@@ -9029,15 +9131,15 @@
         <v>283</v>
       </c>
       <c r="V10" s="23" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="11" spans="2:22" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="151" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C11" s="218" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D11" s="218"/>
       <c r="E11" s="218"/>
@@ -9058,10 +9160,10 @@
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="144" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C12" s="220" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D12" s="220"/>
       <c r="E12" s="220"/>
@@ -9073,17 +9175,17 @@
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="152" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C15" s="159"/>
       <c r="D15" s="159"/>
       <c r="E15" s="210" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="F15" s="211"/>
       <c r="G15" s="212"/>
@@ -9091,7 +9193,7 @@
       <c r="I15" s="159"/>
       <c r="J15" s="160"/>
       <c r="L15" s="213" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="M15" s="213"/>
       <c r="N15" s="213"/>
@@ -9105,55 +9207,55 @@
         <v>1</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>243</v>
       </c>
       <c r="E16" s="164" t="s">
+        <v>559</v>
+      </c>
+      <c r="F16" s="164" t="s">
         <v>560</v>
       </c>
-      <c r="F16" s="164" t="s">
+      <c r="G16" s="164" t="s">
         <v>561</v>
       </c>
-      <c r="G16" s="164" t="s">
-        <v>562</v>
-      </c>
       <c r="H16" s="155" t="s">
+        <v>559</v>
+      </c>
+      <c r="I16" s="155" t="s">
         <v>560</v>
       </c>
-      <c r="I16" s="155" t="s">
+      <c r="J16" s="156" t="s">
         <v>561</v>
       </c>
-      <c r="J16" s="156" t="s">
-        <v>562</v>
-      </c>
       <c r="L16" s="11" t="s">
+        <v>650</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>651</v>
+      </c>
+      <c r="N16" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="O16" s="11" t="s">
         <v>653</v>
       </c>
-      <c r="N16" s="11" t="s">
+      <c r="P16" s="11" t="s">
         <v>654</v>
       </c>
-      <c r="O16" s="11" t="s">
+      <c r="Q16" s="11" t="s">
         <v>655</v>
       </c>
-      <c r="P16" s="11" t="s">
+      <c r="R16" s="11" t="s">
         <v>656</v>
       </c>
-      <c r="Q16" s="11" t="s">
+      <c r="S16" s="182" t="s">
+        <v>756</v>
+      </c>
+      <c r="U16" s="222" t="s">
         <v>657</v>
-      </c>
-      <c r="R16" s="11" t="s">
-        <v>658</v>
-      </c>
-      <c r="S16" s="182" t="s">
-        <v>758</v>
-      </c>
-      <c r="U16" s="222" t="s">
-        <v>659</v>
       </c>
       <c r="V16" s="222"/>
     </row>
@@ -9164,13 +9266,13 @@
       </c>
       <c r="D17" s="31"/>
       <c r="E17" s="165" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="F17" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G17" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H17" s="157" t="str">
         <f>CONCATENATE("0x",BIN2HEX(RIGHT(E17,LEN(E17)-2),2))</f>
@@ -9185,7 +9287,7 @@
         <v>0x03</v>
       </c>
       <c r="K17" s="161" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="L17" s="11" t="str">
         <f>INDEX($V$18:$V$25,MATCH(LEFT(RIGHT(E17,LEN(E17)-2-3),3),$U$18:$U$25,0))</f>
@@ -9216,7 +9318,7 @@
         <v>3-lead amperometric</v>
       </c>
       <c r="U17" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
@@ -9225,7 +9327,7 @@
         <v>433</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E18" s="166"/>
       <c r="F18" s="166"/>
@@ -9234,16 +9336,16 @@
       <c r="I18" s="31"/>
       <c r="J18" s="32"/>
       <c r="U18" s="153" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="V18" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="216"/>
       <c r="C19" s="35" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D19" s="35"/>
       <c r="E19" s="167"/>
@@ -9253,10 +9355,10 @@
       <c r="I19" s="35"/>
       <c r="J19" s="36"/>
       <c r="U19" s="153" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="V19" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="20" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9264,34 +9366,34 @@
         <v>2</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D20" s="28" t="s">
         <v>243</v>
       </c>
       <c r="E20" s="164" t="s">
+        <v>559</v>
+      </c>
+      <c r="F20" s="164" t="s">
         <v>560</v>
       </c>
-      <c r="F20" s="164" t="s">
+      <c r="G20" s="164" t="s">
         <v>561</v>
       </c>
-      <c r="G20" s="164" t="s">
-        <v>562</v>
-      </c>
       <c r="H20" s="155" t="s">
+        <v>559</v>
+      </c>
+      <c r="I20" s="155" t="s">
         <v>560</v>
       </c>
-      <c r="I20" s="155" t="s">
+      <c r="J20" s="156" t="s">
         <v>561</v>
       </c>
-      <c r="J20" s="156" t="s">
-        <v>562</v>
-      </c>
       <c r="U20" s="153" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="V20" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="21" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9300,16 +9402,16 @@
         <v>424</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E21" s="166" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F21" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G21" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H21" s="157" t="str">
         <f>CONCATENATE("0x",BIN2HEX(RIGHT(E21,LEN(E21)-2),2))</f>
@@ -9324,7 +9426,7 @@
         <v>0x03</v>
       </c>
       <c r="K21" s="161" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="L21" s="11" t="str">
         <f>INDEX($V$18:$V$25,MATCH(LEFT(RIGHT(E21,LEN(E21)-2-3),3),$U$18:$U$25,0))</f>
@@ -9355,13 +9457,13 @@
         <v>3-lead amperometric</v>
       </c>
       <c r="S21" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="U21" s="153" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="V21" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="22" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9373,13 +9475,13 @@
         <v>223</v>
       </c>
       <c r="E22" s="166" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F22" s="166" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G22" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H22" s="157" t="str">
         <f t="shared" ref="H22:H26" si="0">CONCATENATE("0x",BIN2HEX(RIGHT(E22,LEN(E22)-2),2))</f>
@@ -9394,7 +9496,7 @@
         <v>0x03</v>
       </c>
       <c r="K22" s="161" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="L22" s="11" t="str">
         <f t="shared" ref="L22:L27" si="3">INDEX($V$18:$V$25,MATCH(LEFT(RIGHT(E22,LEN(E22)-2-3),3),$U$18:$U$25,0))</f>
@@ -9425,13 +9527,13 @@
         <v>3-lead amperometric</v>
       </c>
       <c r="S22" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="U22" s="153" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="V22" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="23" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9440,16 +9542,16 @@
         <v>426</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E23" s="166" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F23" s="166" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G23" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H23" s="157" t="str">
         <f t="shared" si="0"/>
@@ -9464,7 +9566,7 @@
         <v>0x03</v>
       </c>
       <c r="K23" s="161" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="L23" s="11" t="str">
         <f t="shared" si="3"/>
@@ -9495,13 +9597,13 @@
         <v>3-lead amperometric</v>
       </c>
       <c r="S23" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="U23" s="153" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="V23" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="24" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9510,16 +9612,16 @@
         <v>427</v>
       </c>
       <c r="D24" s="87" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E24" s="168" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="F24" s="168" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="G24" s="176" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H24" s="177" t="str">
         <f t="shared" si="0"/>
@@ -9534,7 +9636,7 @@
         <v>0x03</v>
       </c>
       <c r="K24" s="179" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="L24" s="180" t="str">
         <f t="shared" si="3"/>
@@ -9565,13 +9667,13 @@
         <v>3-lead amperometric</v>
       </c>
       <c r="S24" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="U24" s="153" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="V24" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="25" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9580,16 +9682,16 @@
         <v>428</v>
       </c>
       <c r="D25" s="87" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E25" s="166" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="F25" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G25" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H25" s="157" t="str">
         <f t="shared" si="0"/>
@@ -9604,7 +9706,7 @@
         <v>0x03</v>
       </c>
       <c r="K25" s="161" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="L25" s="11" t="str">
         <f t="shared" si="3"/>
@@ -9635,13 +9737,13 @@
         <v>3-lead amperometric</v>
       </c>
       <c r="S25" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="U25" s="153" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="V25" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="26" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9650,16 +9752,16 @@
         <v>429</v>
       </c>
       <c r="D26" s="87" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E26" s="166" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="F26" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G26" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H26" s="157" t="str">
         <f t="shared" si="0"/>
@@ -9674,7 +9776,7 @@
         <v>0x03</v>
       </c>
       <c r="K26" s="161" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="L26" s="11" t="str">
         <f t="shared" si="3"/>
@@ -9705,10 +9807,10 @@
         <v>3-lead amperometric</v>
       </c>
       <c r="S26" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="U26" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="27" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9717,16 +9819,16 @@
         <v>430</v>
       </c>
       <c r="D27" s="87" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="E27" s="166" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="F27" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G27" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H27" s="157" t="str">
         <f t="shared" ref="H27" si="10">CONCATENATE("0x",BIN2HEX(RIGHT(E27,LEN(E27)-2),2))</f>
@@ -9741,7 +9843,7 @@
         <v>0x03</v>
       </c>
       <c r="K27" s="161" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="L27" s="11" t="str">
         <f t="shared" si="3"/>
@@ -9772,10 +9874,10 @@
         <v>3-lead amperometric</v>
       </c>
       <c r="U27" s="153" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="V27" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="28" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9784,7 +9886,7 @@
         <v>431</v>
       </c>
       <c r="D28" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E28" s="157"/>
       <c r="F28" s="157"/>
@@ -9801,10 +9903,10 @@
       <c r="Q28" s="154"/>
       <c r="R28" s="11"/>
       <c r="U28" s="153" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="V28" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="29" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9813,7 +9915,7 @@
         <v>433</v>
       </c>
       <c r="D29" s="166" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E29" s="166"/>
       <c r="F29" s="166"/>
@@ -9830,10 +9932,10 @@
       <c r="Q29" s="154"/>
       <c r="R29" s="11"/>
       <c r="U29" s="153" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="V29" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="30" spans="2:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9842,7 +9944,7 @@
         <v>434</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E30" s="162"/>
       <c r="F30" s="162"/>
@@ -9859,10 +9961,10 @@
       <c r="Q30" s="154"/>
       <c r="R30" s="11"/>
       <c r="U30" s="153" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="V30" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.25">
@@ -9870,28 +9972,28 @@
         <v>3</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D31" s="28" t="s">
         <v>243</v>
       </c>
       <c r="E31" s="164" t="s">
+        <v>559</v>
+      </c>
+      <c r="F31" s="164" t="s">
         <v>560</v>
       </c>
-      <c r="F31" s="164" t="s">
+      <c r="G31" s="164" t="s">
         <v>561</v>
       </c>
-      <c r="G31" s="164" t="s">
-        <v>562</v>
-      </c>
       <c r="H31" s="155" t="s">
+        <v>559</v>
+      </c>
+      <c r="I31" s="155" t="s">
         <v>560</v>
       </c>
-      <c r="I31" s="155" t="s">
+      <c r="J31" s="156" t="s">
         <v>561</v>
-      </c>
-      <c r="J31" s="156" t="s">
-        <v>562</v>
       </c>
       <c r="K31" s="10"/>
       <c r="L31" s="137"/>
@@ -9902,7 +10004,7 @@
       <c r="Q31" s="191"/>
       <c r="R31" s="137"/>
       <c r="U31" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
@@ -9911,16 +10013,16 @@
         <v>424</v>
       </c>
       <c r="D32" s="81" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E32" s="166" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F32" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G32" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H32" s="157" t="str">
         <f>CONCATENATE("0x",BIN2HEX(RIGHT(E32,LEN(E32)-2),2))</f>
@@ -9943,10 +10045,10 @@
       <c r="Q32" s="191"/>
       <c r="R32" s="137"/>
       <c r="U32" s="153" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="V32" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.25">
@@ -9958,13 +10060,13 @@
         <v>223</v>
       </c>
       <c r="E33" s="166" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F33" s="166" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G33" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H33" s="157" t="str">
         <f t="shared" ref="H33:H37" si="13">CONCATENATE("0x",BIN2HEX(RIGHT(E33,LEN(E33)-2),2))</f>
@@ -9987,10 +10089,10 @@
       <c r="Q33" s="191"/>
       <c r="R33" s="137"/>
       <c r="U33" s="153" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="V33" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.25">
@@ -9999,16 +10101,16 @@
         <v>426</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E34" s="166" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F34" s="166" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G34" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H34" s="157" t="str">
         <f t="shared" si="13"/>
@@ -10031,7 +10133,7 @@
       <c r="Q34" s="191"/>
       <c r="R34" s="137"/>
       <c r="U34" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.25">
@@ -10040,16 +10142,16 @@
         <v>427</v>
       </c>
       <c r="D35" s="87" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E35" s="168" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="F35" s="168" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="G35" s="176" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H35" s="177" t="str">
         <f t="shared" si="13"/>
@@ -10072,10 +10174,10 @@
       <c r="Q35" s="10"/>
       <c r="R35" s="10"/>
       <c r="U35" s="153" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="V35" s="141" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.25">
@@ -10084,16 +10186,16 @@
         <v>428</v>
       </c>
       <c r="D36" s="87" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E36" s="166" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="F36" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G36" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H36" s="157" t="str">
         <f t="shared" si="13"/>
@@ -10116,10 +10218,10 @@
       <c r="Q36" s="10"/>
       <c r="R36" s="10"/>
       <c r="U36" s="153" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="V36" s="141" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
@@ -10128,16 +10230,16 @@
         <v>429</v>
       </c>
       <c r="D37" s="87" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E37" s="166" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="F37" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G37" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H37" s="157" t="str">
         <f t="shared" si="13"/>
@@ -10160,10 +10262,10 @@
       <c r="Q37" s="10"/>
       <c r="R37" s="10"/>
       <c r="U37" s="153" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="V37" s="141" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
@@ -10172,12 +10274,12 @@
         <v>430</v>
       </c>
       <c r="D38" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
       <c r="G38" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H38" s="157"/>
       <c r="I38" s="157"/>
@@ -10191,10 +10293,10 @@
       <c r="Q38" s="10"/>
       <c r="R38" s="10"/>
       <c r="U38" s="153" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="V38" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.25">
@@ -10203,12 +10305,12 @@
         <v>431</v>
       </c>
       <c r="D39" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E39" s="137"/>
       <c r="F39" s="137"/>
       <c r="G39" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H39" s="157"/>
       <c r="I39" s="157"/>
@@ -10222,7 +10324,7 @@
       <c r="Q39" s="10"/>
       <c r="R39" s="10"/>
       <c r="U39" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.25">
@@ -10231,7 +10333,7 @@
         <v>433</v>
       </c>
       <c r="D40" s="166" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E40" s="166"/>
       <c r="F40" s="166"/>
@@ -10248,10 +10350,10 @@
       <c r="Q40" s="10"/>
       <c r="R40" s="10"/>
       <c r="U40" s="153" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="V40" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="41" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10260,12 +10362,12 @@
         <v>434</v>
       </c>
       <c r="D41" s="35" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E41" s="193"/>
       <c r="F41" s="193"/>
       <c r="G41" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H41" s="162"/>
       <c r="I41" s="162"/>
@@ -10279,10 +10381,10 @@
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
       <c r="U41" s="153" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="V41" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.25">
@@ -10290,28 +10392,28 @@
         <v>4</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D42" s="28" t="s">
         <v>243</v>
       </c>
       <c r="E42" s="164" t="s">
+        <v>559</v>
+      </c>
+      <c r="F42" s="164" t="s">
         <v>560</v>
       </c>
-      <c r="F42" s="164" t="s">
+      <c r="G42" s="164" t="s">
         <v>561</v>
       </c>
-      <c r="G42" s="164" t="s">
-        <v>562</v>
-      </c>
       <c r="H42" s="155" t="s">
+        <v>559</v>
+      </c>
+      <c r="I42" s="155" t="s">
         <v>560</v>
       </c>
-      <c r="I42" s="155" t="s">
+      <c r="J42" s="156" t="s">
         <v>561</v>
-      </c>
-      <c r="J42" s="156" t="s">
-        <v>562</v>
       </c>
       <c r="K42" s="10"/>
       <c r="L42" s="190"/>
@@ -10322,7 +10424,7 @@
       <c r="Q42" s="10"/>
       <c r="R42" s="10"/>
       <c r="U42" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
@@ -10331,16 +10433,16 @@
         <v>424</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E43" s="166" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F43" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G43" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H43" s="157" t="str">
         <f>CONCATENATE("0x",BIN2HEX(RIGHT(E43,LEN(E43)-2),2))</f>
@@ -10363,7 +10465,7 @@
       <c r="Q43" s="183"/>
       <c r="R43" s="183"/>
       <c r="U43" s="153" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="V43" s="141">
         <v>0</v>
@@ -10378,13 +10480,13 @@
         <v>223</v>
       </c>
       <c r="E44" s="166" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F44" s="166" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G44" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H44" s="157" t="str">
         <f t="shared" ref="H44" si="16">CONCATENATE("0x",BIN2HEX(RIGHT(E44,LEN(E44)-2),2))</f>
@@ -10407,7 +10509,7 @@
       <c r="Q44" s="183"/>
       <c r="R44" s="183"/>
       <c r="U44" s="153" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="V44" s="141">
         <v>0.01</v>
@@ -10419,12 +10521,12 @@
         <v>426</v>
       </c>
       <c r="D45" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
       <c r="G45" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H45" s="157"/>
       <c r="I45" s="157"/>
@@ -10438,7 +10540,7 @@
       <c r="Q45" s="183"/>
       <c r="R45" s="183"/>
       <c r="U45" s="153" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="V45" s="141">
         <v>0.02</v>
@@ -10450,12 +10552,12 @@
         <v>427</v>
       </c>
       <c r="D46" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E46" s="87"/>
       <c r="F46" s="87"/>
       <c r="G46" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H46" s="177"/>
       <c r="I46" s="177"/>
@@ -10469,7 +10571,7 @@
       <c r="Q46" s="183"/>
       <c r="R46" s="183"/>
       <c r="U46" s="153" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="V46" s="141">
         <v>0.04</v>
@@ -10481,12 +10583,12 @@
         <v>428</v>
       </c>
       <c r="D47" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
       <c r="G47" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H47" s="157"/>
       <c r="I47" s="157"/>
@@ -10500,7 +10602,7 @@
       <c r="Q47" s="183"/>
       <c r="R47" s="183"/>
       <c r="U47" s="153" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="V47" s="141">
         <v>0.06</v>
@@ -10512,12 +10614,12 @@
         <v>429</v>
       </c>
       <c r="D48" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
       <c r="G48" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H48" s="157"/>
       <c r="I48" s="157"/>
@@ -10531,7 +10633,7 @@
       <c r="Q48" s="183"/>
       <c r="R48" s="183"/>
       <c r="U48" s="153" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="V48" s="141">
         <v>0.08</v>
@@ -10543,12 +10645,12 @@
         <v>430</v>
       </c>
       <c r="D49" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
       <c r="G49" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H49" s="157"/>
       <c r="I49" s="157"/>
@@ -10562,7 +10664,7 @@
       <c r="Q49" s="183"/>
       <c r="R49" s="183"/>
       <c r="U49" s="153" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="V49" s="141">
         <v>0.1</v>
@@ -10574,12 +10676,12 @@
         <v>431</v>
       </c>
       <c r="D50" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E50" s="137"/>
       <c r="F50" s="137"/>
       <c r="G50" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H50" s="157"/>
       <c r="I50" s="157"/>
@@ -10593,7 +10695,7 @@
       <c r="Q50" s="183"/>
       <c r="R50" s="183"/>
       <c r="U50" s="153" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="V50" s="141">
         <v>0.12</v>
@@ -10605,7 +10707,7 @@
         <v>433</v>
       </c>
       <c r="D51" s="166" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E51" s="166"/>
       <c r="F51" s="166"/>
@@ -10622,7 +10724,7 @@
       <c r="Q51" s="183"/>
       <c r="R51" s="183"/>
       <c r="U51" s="153" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="V51" s="141">
         <v>0.14000000000000001</v>
@@ -10634,12 +10736,12 @@
         <v>434</v>
       </c>
       <c r="D52" s="35" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E52" s="193"/>
       <c r="F52" s="193"/>
       <c r="G52" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H52" s="162"/>
       <c r="I52" s="162"/>
@@ -10653,7 +10755,7 @@
       <c r="Q52" s="183"/>
       <c r="R52" s="183"/>
       <c r="U52" s="153" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="V52" s="141">
         <v>0.16</v>
@@ -10664,28 +10766,28 @@
         <v>5</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D53" s="28" t="s">
         <v>243</v>
       </c>
       <c r="E53" s="164" t="s">
+        <v>559</v>
+      </c>
+      <c r="F53" s="164" t="s">
         <v>560</v>
       </c>
-      <c r="F53" s="164" t="s">
+      <c r="G53" s="164" t="s">
         <v>561</v>
       </c>
-      <c r="G53" s="164" t="s">
-        <v>562</v>
-      </c>
       <c r="H53" s="155" t="s">
+        <v>559</v>
+      </c>
+      <c r="I53" s="155" t="s">
         <v>560</v>
       </c>
-      <c r="I53" s="155" t="s">
+      <c r="J53" s="156" t="s">
         <v>561</v>
-      </c>
-      <c r="J53" s="156" t="s">
-        <v>562</v>
       </c>
       <c r="K53" s="183"/>
       <c r="L53" s="183"/>
@@ -10696,7 +10798,7 @@
       <c r="Q53" s="183"/>
       <c r="R53" s="183"/>
       <c r="U53" s="153" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="V53" s="141">
         <v>0.18</v>
@@ -10708,16 +10810,16 @@
         <v>424</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E54" s="166" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F54" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G54" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H54" s="157" t="str">
         <f>CONCATENATE("0x",BIN2HEX(RIGHT(E54,LEN(E54)-2),2))</f>
@@ -10740,7 +10842,7 @@
       <c r="Q54" s="183"/>
       <c r="R54" s="183"/>
       <c r="U54" s="153" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="V54" s="141">
         <v>0.2</v>
@@ -10755,13 +10857,13 @@
         <v>223</v>
       </c>
       <c r="E55" s="166" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F55" s="166" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G55" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H55" s="157" t="str">
         <f t="shared" ref="H55" si="19">CONCATENATE("0x",BIN2HEX(RIGHT(E55,LEN(E55)-2),2))</f>
@@ -10784,7 +10886,7 @@
       <c r="Q55" s="183"/>
       <c r="R55" s="183"/>
       <c r="U55" s="153" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="V55" s="141">
         <v>0.22</v>
@@ -10796,16 +10898,16 @@
         <v>426</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E56" s="166" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F56" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G56" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H56" s="157" t="str">
         <f>CONCATENATE("0x",BIN2HEX(RIGHT(E56,LEN(E56)-2),2))</f>
@@ -10828,7 +10930,7 @@
       <c r="Q56" s="183"/>
       <c r="R56" s="183"/>
       <c r="U56" s="153" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="V56" s="141">
         <v>0.24</v>
@@ -10843,13 +10945,13 @@
         <v>223</v>
       </c>
       <c r="E57" s="166" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F57" s="166" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G57" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H57" s="157" t="str">
         <f t="shared" ref="H57" si="22">CONCATENATE("0x",BIN2HEX(RIGHT(E57,LEN(E57)-2),2))</f>
@@ -10872,7 +10974,7 @@
       <c r="Q57" s="183"/>
       <c r="R57" s="183"/>
       <c r="U57" s="153" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="58" spans="2:22" x14ac:dyDescent="0.25">
@@ -10881,12 +10983,12 @@
         <v>428</v>
       </c>
       <c r="D58" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
       <c r="G58" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H58" s="157"/>
       <c r="I58" s="157"/>
@@ -10900,10 +11002,10 @@
       <c r="Q58" s="183"/>
       <c r="R58" s="183"/>
       <c r="U58" s="153" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="V58" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="59" spans="2:22" x14ac:dyDescent="0.25">
@@ -10912,12 +11014,12 @@
         <v>429</v>
       </c>
       <c r="D59" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
       <c r="G59" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H59" s="157"/>
       <c r="I59" s="157"/>
@@ -10931,10 +11033,10 @@
       <c r="Q59" s="183"/>
       <c r="R59" s="183"/>
       <c r="U59" s="153" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="V59" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="60" spans="2:22" x14ac:dyDescent="0.25">
@@ -10943,21 +11045,21 @@
         <v>430</v>
       </c>
       <c r="D60" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
       <c r="G60" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H60" s="157"/>
       <c r="I60" s="157"/>
       <c r="J60" s="158"/>
       <c r="U60" s="153" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="V60" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="61" spans="2:22" x14ac:dyDescent="0.25">
@@ -10966,21 +11068,21 @@
         <v>431</v>
       </c>
       <c r="D61" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E61" s="137"/>
       <c r="F61" s="137"/>
       <c r="G61" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H61" s="157"/>
       <c r="I61" s="157"/>
       <c r="J61" s="158"/>
       <c r="U61" s="153" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="V61" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="62" spans="2:22" x14ac:dyDescent="0.25">
@@ -10989,7 +11091,7 @@
         <v>433</v>
       </c>
       <c r="D62" s="166" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E62" s="166"/>
       <c r="F62" s="166"/>
@@ -10998,10 +11100,10 @@
       <c r="I62" s="157"/>
       <c r="J62" s="158"/>
       <c r="U62" s="153" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="V62" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="63" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11010,21 +11112,21 @@
         <v>434</v>
       </c>
       <c r="D63" s="35" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E63" s="193"/>
       <c r="F63" s="193"/>
       <c r="G63" s="194" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H63" s="162"/>
       <c r="I63" s="162"/>
       <c r="J63" s="163"/>
       <c r="U63" s="153" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="V63" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="64" spans="2:22" x14ac:dyDescent="0.25">
@@ -11032,28 +11134,28 @@
         <v>6</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D64" s="28" t="s">
         <v>243</v>
       </c>
       <c r="E64" s="164" t="s">
+        <v>559</v>
+      </c>
+      <c r="F64" s="164" t="s">
         <v>560</v>
       </c>
-      <c r="F64" s="164" t="s">
+      <c r="G64" s="164" t="s">
         <v>561</v>
       </c>
-      <c r="G64" s="164" t="s">
-        <v>562</v>
-      </c>
       <c r="H64" s="155" t="s">
+        <v>559</v>
+      </c>
+      <c r="I64" s="155" t="s">
         <v>560</v>
       </c>
-      <c r="I64" s="155" t="s">
+      <c r="J64" s="156" t="s">
         <v>561</v>
-      </c>
-      <c r="J64" s="156" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
@@ -11062,16 +11164,16 @@
         <v>424</v>
       </c>
       <c r="D65" s="31" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E65" s="166" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F65" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G65" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H65" s="157" t="str">
         <f>CONCATENATE("0x",BIN2HEX(RIGHT(E65,LEN(E65)-2),2))</f>
@@ -11095,13 +11197,13 @@
         <v>223</v>
       </c>
       <c r="E66" s="166" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F66" s="166" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G66" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H66" s="157" t="str">
         <f t="shared" ref="H66" si="25">CONCATENATE("0x",BIN2HEX(RIGHT(E66,LEN(E66)-2),2))</f>
@@ -11122,16 +11224,16 @@
         <v>426</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="E67" s="166" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F67" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G67" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H67" s="157" t="str">
         <f>CONCATENATE("0x",BIN2HEX(RIGHT(E67,LEN(E67)-2),2))</f>
@@ -11155,13 +11257,13 @@
         <v>223</v>
       </c>
       <c r="E68" s="166" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F68" s="166" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G68" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H68" s="157" t="str">
         <f t="shared" ref="H68" si="28">CONCATENATE("0x",BIN2HEX(RIGHT(E68,LEN(E68)-2),2))</f>
@@ -11182,25 +11284,25 @@
         <v>428</v>
       </c>
       <c r="D69" s="87" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E69" s="166" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="F69" s="166" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G69" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H69" s="157" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I69" s="157" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="J69" s="158" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
@@ -11209,12 +11311,12 @@
         <v>429</v>
       </c>
       <c r="D70" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E70" s="10"/>
       <c r="F70" s="10"/>
       <c r="G70" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H70" s="157"/>
       <c r="I70" s="157"/>
@@ -11226,12 +11328,12 @@
         <v>430</v>
       </c>
       <c r="D71" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E71" s="10"/>
       <c r="F71" s="10"/>
       <c r="G71" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H71" s="157"/>
       <c r="I71" s="157"/>
@@ -11243,12 +11345,12 @@
         <v>431</v>
       </c>
       <c r="D72" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E72" s="137"/>
       <c r="F72" s="137"/>
       <c r="G72" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H72" s="157"/>
       <c r="I72" s="157"/>
@@ -11260,12 +11362,12 @@
         <v>433</v>
       </c>
       <c r="D73" s="87" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E73" s="10"/>
       <c r="F73" s="10"/>
       <c r="G73" s="165" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H73" s="157"/>
       <c r="I73" s="157"/>
@@ -11277,12 +11379,12 @@
         <v>434</v>
       </c>
       <c r="D74" s="35" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E74" s="193"/>
       <c r="F74" s="193"/>
       <c r="G74" s="194" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H74" s="162"/>
       <c r="I74" s="162"/>
@@ -11340,46 +11442,46 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I3" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="P3" s="56" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C5" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D5" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C7" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -11400,24 +11502,24 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C11" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D11" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="E11" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -11431,7 +11533,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C13">
         <v>6</v>
@@ -11445,10 +11547,10 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B14" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C14">
         <v>12</v>
@@ -11462,10 +11564,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B15" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -11479,10 +11581,10 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B16" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C16">
         <v>16</v>
@@ -11496,10 +11598,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B17" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C17">
         <v>18</v>
@@ -11513,10 +11615,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B18" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C18">
         <v>20</v>
@@ -11530,10 +11632,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B19" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C19">
         <v>24</v>
@@ -11547,7 +11649,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C21">
         <f>C18-C14</f>
@@ -11562,7 +11664,7 @@
         <v>1.7125000000000057</v>
       </c>
       <c r="F21" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -11580,15 +11682,15 @@
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
       <c r="D27" s="28" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B28" s="31"/>
       <c r="C28" s="31">
@@ -11603,7 +11705,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="B29" s="31"/>
       <c r="C29" s="31">
@@ -11618,7 +11720,7 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="34" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B30" s="35"/>
       <c r="C30" s="35">
@@ -11634,7 +11736,7 @@
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B32" s="138">
         <v>0.67</v>
@@ -11645,10 +11747,10 @@
     </row>
     <row r="33" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="30" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C33" s="31"/>
       <c r="D33" s="31"/>
@@ -11661,13 +11763,13 @@
       <c r="D34" s="31"/>
       <c r="E34" s="32"/>
       <c r="F34" s="27" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G34" s="28">
         <v>5</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11677,14 +11779,14 @@
       <c r="D35" s="31"/>
       <c r="E35" s="32"/>
       <c r="F35" s="30" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="G35" s="31">
         <f>0.67*G34</f>
         <v>3.35</v>
       </c>
       <c r="H35" s="32" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -11694,23 +11796,23 @@
       <c r="D36" s="31"/>
       <c r="E36" s="32"/>
       <c r="F36" s="30" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="G36" s="31">
         <f>0.2*G34</f>
         <v>1</v>
       </c>
       <c r="H36" s="32" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="J36" s="27" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="K36" s="28">
         <v>5</v>
       </c>
       <c r="L36" s="29" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -11720,23 +11822,23 @@
       <c r="D37" s="31"/>
       <c r="E37" s="32"/>
       <c r="F37" s="30" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="G37" s="139">
         <v>1000000</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="J37" s="30" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="K37" s="31">
         <f>0.2*K36</f>
         <v>1</v>
       </c>
       <c r="L37" s="32" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -11746,24 +11848,24 @@
       <c r="D38" s="31"/>
       <c r="E38" s="32"/>
       <c r="F38" s="30" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="G38" s="139">
         <f>(G36)/G37</f>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="H38" s="32" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="J38" s="30" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K38" s="31">
         <f>0.2*K36</f>
         <v>1</v>
       </c>
       <c r="L38" s="32" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -11778,16 +11880,16 @@
         <v>1</v>
       </c>
       <c r="H39" s="32" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="J39" s="30" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="K39" s="139">
         <v>1000000</v>
       </c>
       <c r="L39" s="32" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -11797,21 +11899,21 @@
       <c r="D40" s="31"/>
       <c r="E40" s="32"/>
       <c r="F40" s="30" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G40" s="31">
         <v>35000</v>
       </c>
       <c r="H40" s="32"/>
       <c r="J40" s="30" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K40" s="139">
         <f>(K38)/K39</f>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="L40" s="32" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
@@ -11821,14 +11923,14 @@
       <c r="D41" s="31"/>
       <c r="E41" s="32"/>
       <c r="F41" s="30" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="G41" s="139">
         <f>G35+G40*G38</f>
         <v>3.3850000000000002</v>
       </c>
       <c r="H41" s="32" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="J41" s="30"/>
       <c r="K41" s="139">
@@ -11836,15 +11938,15 @@
         <v>1</v>
       </c>
       <c r="L41" s="32" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="34" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C42" s="35">
         <v>20</v>
@@ -11864,7 +11966,7 @@
         <v>410</v>
       </c>
       <c r="J42" s="30" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="K42" s="31">
         <v>350000</v>
@@ -11873,14 +11975,14 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J43" s="30" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="K43" s="139">
         <f>K37+K42*K40</f>
         <v>1.35</v>
       </c>
       <c r="L43" s="32" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11896,7 +11998,7 @@
     <row r="47" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="27" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B48" s="28"/>
       <c r="C48" s="28"/>
@@ -11923,22 +12025,22 @@
       <c r="C49" s="31"/>
       <c r="D49" s="31"/>
       <c r="E49" s="164" t="s">
+        <v>559</v>
+      </c>
+      <c r="F49" s="164" t="s">
         <v>560</v>
       </c>
-      <c r="F49" s="164" t="s">
+      <c r="G49" s="164" t="s">
         <v>561</v>
       </c>
-      <c r="G49" s="164" t="s">
-        <v>562</v>
-      </c>
       <c r="H49" s="155" t="s">
+        <v>559</v>
+      </c>
+      <c r="I49" s="155" t="s">
         <v>560</v>
       </c>
-      <c r="I49" s="155" t="s">
+      <c r="J49" s="156" t="s">
         <v>561</v>
-      </c>
-      <c r="J49" s="156" t="s">
-        <v>562</v>
       </c>
       <c r="K49" s="31"/>
       <c r="L49" s="31"/>
@@ -11956,13 +12058,13 @@
       <c r="C50" s="31"/>
       <c r="D50" s="31"/>
       <c r="E50" s="166" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F50" s="166" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="G50" s="165" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H50" s="157" t="str">
         <f t="shared" ref="H50:J50" si="0">CONCATENATE("0x",BIN2HEX(RIGHT(E50,LEN(E50)-2),2))</f>
@@ -11978,25 +12080,25 @@
       </c>
       <c r="K50" s="31"/>
       <c r="L50" s="157" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="M50" s="157" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="N50" s="157" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="O50" s="157" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="P50" s="157" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="Q50" s="171">
         <v>0.12</v>
       </c>
       <c r="R50" s="157" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="S50" s="32"/>
     </row>
@@ -12005,16 +12107,16 @@
       <c r="B51" s="31"/>
       <c r="C51" s="31"/>
       <c r="D51" s="27" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F51" s="28" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="G51" s="28" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="H51" s="28"/>
       <c r="I51" s="28"/>
@@ -12034,34 +12136,34 @@
       <c r="B52" s="31"/>
       <c r="C52" s="31"/>
       <c r="D52" s="27" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="E52" s="169" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="F52" s="169" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="G52" s="169" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="H52" s="169" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="I52" s="169" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J52" s="169" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="K52" s="170" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="L52" s="174" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="M52" s="169" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="N52" s="31"/>
       <c r="O52" s="31"/>
@@ -12075,34 +12177,34 @@
       <c r="B53" s="31"/>
       <c r="C53" s="31"/>
       <c r="D53" s="30" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E53" s="157" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F53" s="157" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="G53" s="31" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="H53" s="31" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="I53" s="31" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="J53" s="31" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="K53" s="32" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="L53" s="135" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="M53" s="10" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="N53" s="31"/>
       <c r="O53" s="31"/>
@@ -12116,7 +12218,7 @@
       <c r="B54" s="31"/>
       <c r="C54" s="31"/>
       <c r="D54" s="30" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E54" s="171">
         <v>-0.12</v>
@@ -12157,7 +12259,7 @@
       <c r="B55" s="31"/>
       <c r="C55" s="31"/>
       <c r="D55" s="30" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E55" s="157">
         <v>-1.002</v>
@@ -12198,7 +12300,7 @@
       <c r="B56" s="31"/>
       <c r="C56" s="31"/>
       <c r="D56" s="185" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E56" s="186"/>
       <c r="F56" s="186"/>
@@ -12545,7 +12647,7 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -12553,7 +12655,7 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -12561,7 +12663,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -12569,7 +12671,7 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -12577,7 +12679,7 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -12585,10 +12687,10 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C23" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -12596,7 +12698,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -12604,7 +12706,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -12612,7 +12714,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -12620,7 +12722,7 @@
         <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -12628,7 +12730,7 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -12636,7 +12738,7 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -12644,7 +12746,7 @@
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -12652,7 +12754,7 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -12660,7 +12762,7 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -12668,7 +12770,7 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -12676,7 +12778,7 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -12684,7 +12786,7 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -12692,7 +12794,7 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -12700,7 +12802,7 @@
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -12708,7 +12810,7 @@
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -12716,7 +12818,7 @@
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -12724,7 +12826,7 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -12732,7 +12834,7 @@
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -12740,7 +12842,7 @@
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -12748,7 +12850,7 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -12756,7 +12858,7 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -12764,7 +12866,7 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -12772,7 +12874,7 @@
         <v>42</v>
       </c>
       <c r="B46" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
   </sheetData>
@@ -12980,7 +13082,7 @@
   <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12996,10 +13098,10 @@
     </row>
     <row r="2" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="58" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -13231,7 +13333,7 @@
         <v>259</v>
       </c>
       <c r="B31" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -13327,7 +13429,7 @@
     </row>
     <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B43" t="s">
         <v>320</v>
@@ -13335,7 +13437,7 @@
     </row>
     <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B44" t="s">
         <v>320</v>
@@ -13343,7 +13445,7 @@
     </row>
     <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B45" t="s">
         <v>320</v>
@@ -13351,7 +13453,7 @@
     </row>
     <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B46" t="s">
         <v>320</v>
@@ -13359,7 +13461,7 @@
     </row>
     <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B47" t="s">
         <v>320</v>
@@ -13367,7 +13469,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -13382,7 +13484,7 @@
     </row>
     <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B51" t="s">
         <v>320</v>
@@ -13390,7 +13492,7 @@
     </row>
     <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B52" t="s">
         <v>320</v>
@@ -13398,12 +13500,12 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B54" t="s">
         <v>369</v>
@@ -13411,39 +13513,39 @@
     </row>
     <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B55" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B56" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B57" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>619</v>
+      </c>
+      <c r="B58" t="s">
         <v>621</v>
-      </c>
-      <c r="B58" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B59" t="s">
         <v>320</v>
@@ -13451,7 +13553,7 @@
     </row>
     <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B60" t="s">
         <v>320</v>
@@ -13459,15 +13561,15 @@
     </row>
     <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="86" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B61" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B62" t="s">
         <v>320</v>
@@ -13475,27 +13577,27 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B67" t="s">
         <v>320</v>
@@ -13503,7 +13605,7 @@
     </row>
     <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="B68" t="s">
         <v>320</v>
@@ -14389,7 +14491,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14431,26 +14533,30 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="122.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="57" t="s">
         <v>181</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>475</v>
       </c>
@@ -14460,26 +14566,45 @@
       <c r="C3" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="223" t="s">
+        <v>781</v>
+      </c>
+      <c r="G3" s="224"/>
+      <c r="H3" s="225"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>473</v>
       </c>
       <c r="D4" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="30" t="s">
+        <v>782</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>792</v>
+      </c>
+      <c r="H4" s="32"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>473</v>
       </c>
       <c r="D5" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="30" t="s">
+        <v>783</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>793</v>
+      </c>
+      <c r="H5" s="32"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -14488,12 +14613,19 @@
         <v>20</v>
       </c>
       <c r="D6" t="s">
+        <v>780</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>784</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>785</v>
+      </c>
+      <c r="H6" s="36"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>479</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>480</v>
       </c>
       <c r="B7">
         <v>1.5</v>
@@ -14502,12 +14634,12 @@
         <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B8">
         <v>0.2</v>
@@ -14516,28 +14648,79 @@
         <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+      <c r="F8" s="223" t="s">
+        <v>786</v>
+      </c>
+      <c r="G8" s="224"/>
+      <c r="H8" s="225"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>480</v>
+      </c>
+      <c r="B9" t="s">
         <v>481</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>482</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>483</v>
       </c>
-      <c r="D9" t="s">
-        <v>484</v>
-      </c>
+      <c r="F9" s="226" t="s">
+        <v>791</v>
+      </c>
+      <c r="G9" s="227"/>
+      <c r="H9" s="228"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="30" t="s">
+        <v>787</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>793</v>
+      </c>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F11" s="30" t="s">
+        <v>788</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>792</v>
+      </c>
+      <c r="H11" s="32"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="30" t="s">
+        <v>789</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>785</v>
+      </c>
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="229" t="s">
+        <v>790</v>
+      </c>
+      <c r="G13" s="230"/>
+      <c r="H13" s="231"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F13:H13"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="Contents!A1" display="Contents!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15421,8 +15604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L101"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35:J42"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I45" sqref="H45:I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15751,7 +15934,7 @@
         <v>283</v>
       </c>
       <c r="J38" s="127" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="39" spans="4:10" x14ac:dyDescent="0.25">
@@ -15762,7 +15945,7 @@
         <v>283</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="40" spans="4:10" x14ac:dyDescent="0.25">
@@ -15773,7 +15956,7 @@
         <v>283</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.25">
@@ -15784,7 +15967,7 @@
         <v>283</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="42" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16508,14 +16691,14 @@
         <v>390</v>
       </c>
       <c r="J9" s="207" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K9" s="208"/>
       <c r="L9" s="94" t="s">
         <v>398</v>
       </c>
       <c r="M9" s="207" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="N9" s="208"/>
       <c r="O9" s="91" t="s">

</xml_diff>

<commit_message>
bulkhead design, updated confsets added 7th
</commit_message>
<xml_diff>
--- a/1-SystemDocs/System_spec_v4.xlsx
+++ b/1-SystemDocs/System_spec_v4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-120" windowWidth="12960" windowHeight="11760" tabRatio="760" firstSheet="12" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="12960" windowHeight="11760" tabRatio="760" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="13" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="795">
   <si>
     <t>ETH*</t>
   </si>
@@ -2516,6 +2516,9 @@
       </rPr>
       <t xml:space="preserve"> cable</t>
     </r>
+  </si>
+  <si>
+    <t>0b11111111</t>
   </si>
 </sst>
 </file>
@@ -3487,6 +3490,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3498,15 +3513,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3522,9 +3528,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4018,11 +4021,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="398040296"/>
-        <c:axId val="398041472"/>
+        <c:axId val="364100120"/>
+        <c:axId val="364094632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="398040296"/>
+        <c:axId val="364100120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -4067,12 +4070,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="398041472"/>
+        <c:crossAx val="364094632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="398041472"/>
+        <c:axId val="364094632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1400"/>
@@ -4131,7 +4134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="398040296"/>
+        <c:crossAx val="364100120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4847,7 +4850,7 @@
         <xdr:cNvPr id="2" name="Obrázok 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8933,10 +8936,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V74"/>
+  <dimension ref="B1:V85"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L82" sqref="L82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8963,19 +8966,19 @@
       </c>
     </row>
     <row r="3" spans="2:22" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="217" t="s">
+      <c r="B3" s="218" t="s">
         <v>536</v>
       </c>
-      <c r="C3" s="217"/>
-      <c r="D3" s="217"/>
-      <c r="E3" s="217"/>
-      <c r="F3" s="217"/>
-      <c r="G3" s="217"/>
-      <c r="H3" s="217"/>
-      <c r="I3" s="217"/>
-      <c r="J3" s="217"/>
-      <c r="K3" s="217"/>
-      <c r="L3" s="217"/>
+      <c r="C3" s="218"/>
+      <c r="D3" s="218"/>
+      <c r="E3" s="218"/>
+      <c r="F3" s="218"/>
+      <c r="G3" s="218"/>
+      <c r="H3" s="218"/>
+      <c r="I3" s="218"/>
+      <c r="J3" s="218"/>
+      <c r="K3" s="218"/>
+      <c r="L3" s="218"/>
       <c r="M3" s="129"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
@@ -9114,16 +9117,16 @@
       <c r="B10" s="151" t="s">
         <v>634</v>
       </c>
-      <c r="C10" s="218" t="s">
+      <c r="C10" s="219" t="s">
         <v>641</v>
       </c>
-      <c r="D10" s="218"/>
-      <c r="E10" s="218"/>
-      <c r="F10" s="218"/>
-      <c r="G10" s="218"/>
-      <c r="H10" s="218"/>
-      <c r="I10" s="218"/>
-      <c r="J10" s="219"/>
+      <c r="D10" s="219"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="219"/>
+      <c r="H10" s="219"/>
+      <c r="I10" s="219"/>
+      <c r="J10" s="220"/>
       <c r="T10" s="22">
         <v>9</v>
       </c>
@@ -9138,16 +9141,16 @@
       <c r="B11" s="151" t="s">
         <v>640</v>
       </c>
-      <c r="C11" s="218" t="s">
+      <c r="C11" s="219" t="s">
         <v>643</v>
       </c>
-      <c r="D11" s="218"/>
-      <c r="E11" s="218"/>
-      <c r="F11" s="218"/>
-      <c r="G11" s="218"/>
-      <c r="H11" s="218"/>
-      <c r="I11" s="218"/>
-      <c r="J11" s="219"/>
+      <c r="D11" s="219"/>
+      <c r="E11" s="219"/>
+      <c r="F11" s="219"/>
+      <c r="G11" s="219"/>
+      <c r="H11" s="219"/>
+      <c r="I11" s="219"/>
+      <c r="J11" s="220"/>
       <c r="T11" s="24" t="s">
         <v>102</v>
       </c>
@@ -9162,16 +9165,16 @@
       <c r="B12" s="144" t="s">
         <v>639</v>
       </c>
-      <c r="C12" s="220" t="s">
+      <c r="C12" s="221" t="s">
         <v>642</v>
       </c>
-      <c r="D12" s="220"/>
-      <c r="E12" s="220"/>
-      <c r="F12" s="220"/>
-      <c r="G12" s="220"/>
-      <c r="H12" s="220"/>
-      <c r="I12" s="220"/>
-      <c r="J12" s="221"/>
+      <c r="D12" s="221"/>
+      <c r="E12" s="221"/>
+      <c r="F12" s="221"/>
+      <c r="G12" s="221"/>
+      <c r="H12" s="221"/>
+      <c r="I12" s="221"/>
+      <c r="J12" s="222"/>
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -9184,26 +9187,26 @@
       </c>
       <c r="C15" s="159"/>
       <c r="D15" s="159"/>
-      <c r="E15" s="210" t="s">
+      <c r="E15" s="214" t="s">
         <v>679</v>
       </c>
-      <c r="F15" s="211"/>
-      <c r="G15" s="212"/>
+      <c r="F15" s="215"/>
+      <c r="G15" s="216"/>
       <c r="H15" s="159"/>
       <c r="I15" s="159"/>
       <c r="J15" s="160"/>
-      <c r="L15" s="213" t="s">
+      <c r="L15" s="217" t="s">
         <v>704</v>
       </c>
-      <c r="M15" s="213"/>
-      <c r="N15" s="213"/>
-      <c r="O15" s="213"/>
-      <c r="P15" s="213"/>
-      <c r="Q15" s="213"/>
-      <c r="R15" s="213"/>
+      <c r="M15" s="217"/>
+      <c r="N15" s="217"/>
+      <c r="O15" s="217"/>
+      <c r="P15" s="217"/>
+      <c r="Q15" s="217"/>
+      <c r="R15" s="217"/>
     </row>
     <row r="16" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="214">
+      <c r="B16" s="210">
         <v>1</v>
       </c>
       <c r="C16" s="28" t="s">
@@ -9254,13 +9257,13 @@
       <c r="S16" s="182" t="s">
         <v>756</v>
       </c>
-      <c r="U16" s="222" t="s">
+      <c r="U16" s="213" t="s">
         <v>657</v>
       </c>
-      <c r="V16" s="222"/>
+      <c r="V16" s="213"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="215"/>
+      <c r="B17" s="211"/>
       <c r="C17" s="31" t="s">
         <v>428</v>
       </c>
@@ -9322,7 +9325,7 @@
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="215"/>
+      <c r="B18" s="211"/>
       <c r="C18" s="31" t="s">
         <v>433</v>
       </c>
@@ -9343,7 +9346,7 @@
       </c>
     </row>
     <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="216"/>
+      <c r="B19" s="212"/>
       <c r="C19" s="35" t="s">
         <v>646</v>
       </c>
@@ -9362,7 +9365,7 @@
       </c>
     </row>
     <row r="20" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="214">
+      <c r="B20" s="210">
         <v>2</v>
       </c>
       <c r="C20" s="28" t="s">
@@ -9397,7 +9400,7 @@
       </c>
     </row>
     <row r="21" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="215"/>
+      <c r="B21" s="211"/>
       <c r="C21" s="31" t="s">
         <v>424</v>
       </c>
@@ -9467,7 +9470,7 @@
       </c>
     </row>
     <row r="22" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="215"/>
+      <c r="B22" s="211"/>
       <c r="C22" s="31" t="s">
         <v>425</v>
       </c>
@@ -9537,7 +9540,7 @@
       </c>
     </row>
     <row r="23" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="215"/>
+      <c r="B23" s="211"/>
       <c r="C23" s="31" t="s">
         <v>426</v>
       </c>
@@ -9607,7 +9610,7 @@
       </c>
     </row>
     <row r="24" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="215"/>
+      <c r="B24" s="211"/>
       <c r="C24" s="81" t="s">
         <v>427</v>
       </c>
@@ -9677,7 +9680,7 @@
       </c>
     </row>
     <row r="25" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="215"/>
+      <c r="B25" s="211"/>
       <c r="C25" s="31" t="s">
         <v>428</v>
       </c>
@@ -9747,7 +9750,7 @@
       </c>
     </row>
     <row r="26" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="215"/>
+      <c r="B26" s="211"/>
       <c r="C26" s="31" t="s">
         <v>429</v>
       </c>
@@ -9814,7 +9817,7 @@
       </c>
     </row>
     <row r="27" spans="2:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="215"/>
+      <c r="B27" s="211"/>
       <c r="C27" s="81" t="s">
         <v>430</v>
       </c>
@@ -9881,7 +9884,7 @@
       </c>
     </row>
     <row r="28" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="215"/>
+      <c r="B28" s="211"/>
       <c r="C28" s="31" t="s">
         <v>431</v>
       </c>
@@ -9910,7 +9913,7 @@
       </c>
     </row>
     <row r="29" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="215"/>
+      <c r="B29" s="211"/>
       <c r="C29" s="31" t="s">
         <v>433</v>
       </c>
@@ -9919,7 +9922,9 @@
       </c>
       <c r="E29" s="166"/>
       <c r="F29" s="166"/>
-      <c r="G29" s="166"/>
+      <c r="G29" s="165" t="s">
+        <v>794</v>
+      </c>
       <c r="H29" s="157"/>
       <c r="I29" s="157"/>
       <c r="J29" s="158"/>
@@ -9939,7 +9944,7 @@
       </c>
     </row>
     <row r="30" spans="2:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="216"/>
+      <c r="B30" s="212"/>
       <c r="C30" s="35" t="s">
         <v>434</v>
       </c>
@@ -9968,7 +9973,7 @@
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="214">
+      <c r="B31" s="210">
         <v>3</v>
       </c>
       <c r="C31" s="28" t="s">
@@ -10008,7 +10013,7 @@
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B32" s="215"/>
+      <c r="B32" s="211"/>
       <c r="C32" s="31" t="s">
         <v>424</v>
       </c>
@@ -10052,7 +10057,7 @@
       </c>
     </row>
     <row r="33" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B33" s="215"/>
+      <c r="B33" s="211"/>
       <c r="C33" s="31" t="s">
         <v>425</v>
       </c>
@@ -10096,7 +10101,7 @@
       </c>
     </row>
     <row r="34" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B34" s="215"/>
+      <c r="B34" s="211"/>
       <c r="C34" s="31" t="s">
         <v>426</v>
       </c>
@@ -10137,7 +10142,7 @@
       </c>
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B35" s="215"/>
+      <c r="B35" s="211"/>
       <c r="C35" s="81" t="s">
         <v>427</v>
       </c>
@@ -10181,7 +10186,7 @@
       </c>
     </row>
     <row r="36" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B36" s="215"/>
+      <c r="B36" s="211"/>
       <c r="C36" s="31" t="s">
         <v>428</v>
       </c>
@@ -10225,7 +10230,7 @@
       </c>
     </row>
     <row r="37" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B37" s="215"/>
+      <c r="B37" s="211"/>
       <c r="C37" s="31" t="s">
         <v>429</v>
       </c>
@@ -10269,7 +10274,7 @@
       </c>
     </row>
     <row r="38" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B38" s="215"/>
+      <c r="B38" s="211"/>
       <c r="C38" s="81" t="s">
         <v>430</v>
       </c>
@@ -10300,7 +10305,7 @@
       </c>
     </row>
     <row r="39" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B39" s="215"/>
+      <c r="B39" s="211"/>
       <c r="C39" s="31" t="s">
         <v>431</v>
       </c>
@@ -10328,7 +10333,7 @@
       </c>
     </row>
     <row r="40" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B40" s="215"/>
+      <c r="B40" s="211"/>
       <c r="C40" s="31" t="s">
         <v>433</v>
       </c>
@@ -10337,7 +10342,9 @@
       </c>
       <c r="E40" s="166"/>
       <c r="F40" s="166"/>
-      <c r="G40" s="166"/>
+      <c r="G40" s="165" t="s">
+        <v>794</v>
+      </c>
       <c r="H40" s="157"/>
       <c r="I40" s="157"/>
       <c r="J40" s="158"/>
@@ -10357,7 +10364,7 @@
       </c>
     </row>
     <row r="41" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="216"/>
+      <c r="B41" s="212"/>
       <c r="C41" s="35" t="s">
         <v>434</v>
       </c>
@@ -10388,7 +10395,7 @@
       </c>
     </row>
     <row r="42" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B42" s="214">
+      <c r="B42" s="210">
         <v>4</v>
       </c>
       <c r="C42" s="28" t="s">
@@ -10428,7 +10435,7 @@
       </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B43" s="215"/>
+      <c r="B43" s="211"/>
       <c r="C43" s="31" t="s">
         <v>424</v>
       </c>
@@ -10472,7 +10479,7 @@
       </c>
     </row>
     <row r="44" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B44" s="215"/>
+      <c r="B44" s="211"/>
       <c r="C44" s="31" t="s">
         <v>425</v>
       </c>
@@ -10516,7 +10523,7 @@
       </c>
     </row>
     <row r="45" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B45" s="215"/>
+      <c r="B45" s="211"/>
       <c r="C45" s="31" t="s">
         <v>426</v>
       </c>
@@ -10547,7 +10554,7 @@
       </c>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B46" s="215"/>
+      <c r="B46" s="211"/>
       <c r="C46" s="81" t="s">
         <v>427</v>
       </c>
@@ -10578,7 +10585,7 @@
       </c>
     </row>
     <row r="47" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B47" s="215"/>
+      <c r="B47" s="211"/>
       <c r="C47" s="31" t="s">
         <v>428</v>
       </c>
@@ -10609,7 +10616,7 @@
       </c>
     </row>
     <row r="48" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B48" s="215"/>
+      <c r="B48" s="211"/>
       <c r="C48" s="31" t="s">
         <v>429</v>
       </c>
@@ -10640,7 +10647,7 @@
       </c>
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B49" s="215"/>
+      <c r="B49" s="211"/>
       <c r="C49" s="81" t="s">
         <v>430</v>
       </c>
@@ -10671,7 +10678,7 @@
       </c>
     </row>
     <row r="50" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B50" s="215"/>
+      <c r="B50" s="211"/>
       <c r="C50" s="31" t="s">
         <v>431</v>
       </c>
@@ -10702,7 +10709,7 @@
       </c>
     </row>
     <row r="51" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B51" s="215"/>
+      <c r="B51" s="211"/>
       <c r="C51" s="31" t="s">
         <v>433</v>
       </c>
@@ -10711,7 +10718,9 @@
       </c>
       <c r="E51" s="166"/>
       <c r="F51" s="166"/>
-      <c r="G51" s="166"/>
+      <c r="G51" s="165" t="s">
+        <v>794</v>
+      </c>
       <c r="H51" s="157"/>
       <c r="I51" s="157"/>
       <c r="J51" s="158"/>
@@ -10731,7 +10740,7 @@
       </c>
     </row>
     <row r="52" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="216"/>
+      <c r="B52" s="212"/>
       <c r="C52" s="35" t="s">
         <v>434</v>
       </c>
@@ -10762,7 +10771,7 @@
       </c>
     </row>
     <row r="53" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B53" s="214">
+      <c r="B53" s="210">
         <v>5</v>
       </c>
       <c r="C53" s="28" t="s">
@@ -10805,7 +10814,7 @@
       </c>
     </row>
     <row r="54" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B54" s="215"/>
+      <c r="B54" s="211"/>
       <c r="C54" s="31" t="s">
         <v>424</v>
       </c>
@@ -10849,7 +10858,7 @@
       </c>
     </row>
     <row r="55" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B55" s="215"/>
+      <c r="B55" s="211"/>
       <c r="C55" s="31" t="s">
         <v>425</v>
       </c>
@@ -10893,7 +10902,7 @@
       </c>
     </row>
     <row r="56" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B56" s="215"/>
+      <c r="B56" s="211"/>
       <c r="C56" s="31" t="s">
         <v>426</v>
       </c>
@@ -10937,7 +10946,7 @@
       </c>
     </row>
     <row r="57" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B57" s="215"/>
+      <c r="B57" s="211"/>
       <c r="C57" s="81" t="s">
         <v>427</v>
       </c>
@@ -10962,7 +10971,7 @@
         <v>0x40</v>
       </c>
       <c r="J57" s="158" t="str">
-        <f t="shared" ref="J57" si="24">CONCATENATE("0x",BIN2HEX(RIGHT(G57,LEN(G57)-2),2))</f>
+        <f t="shared" ref="J57:J63" si="24">CONCATENATE("0x",BIN2HEX(RIGHT(G57,LEN(G57)-2),2))</f>
         <v>0x03</v>
       </c>
       <c r="K57" s="183"/>
@@ -10978,7 +10987,7 @@
       </c>
     </row>
     <row r="58" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B58" s="215"/>
+      <c r="B58" s="211"/>
       <c r="C58" s="31" t="s">
         <v>428</v>
       </c>
@@ -10992,7 +11001,10 @@
       </c>
       <c r="H58" s="157"/>
       <c r="I58" s="157"/>
-      <c r="J58" s="158"/>
+      <c r="J58" s="158" t="str">
+        <f t="shared" si="24"/>
+        <v>0x00</v>
+      </c>
       <c r="K58" s="183"/>
       <c r="L58" s="183"/>
       <c r="M58" s="183"/>
@@ -11009,7 +11021,7 @@
       </c>
     </row>
     <row r="59" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B59" s="215"/>
+      <c r="B59" s="211"/>
       <c r="C59" s="31" t="s">
         <v>429</v>
       </c>
@@ -11023,7 +11035,10 @@
       </c>
       <c r="H59" s="157"/>
       <c r="I59" s="157"/>
-      <c r="J59" s="158"/>
+      <c r="J59" s="158" t="str">
+        <f t="shared" si="24"/>
+        <v>0x00</v>
+      </c>
       <c r="K59" s="183"/>
       <c r="L59" s="183"/>
       <c r="M59" s="183"/>
@@ -11040,7 +11055,7 @@
       </c>
     </row>
     <row r="60" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B60" s="215"/>
+      <c r="B60" s="211"/>
       <c r="C60" s="81" t="s">
         <v>430</v>
       </c>
@@ -11054,7 +11069,10 @@
       </c>
       <c r="H60" s="157"/>
       <c r="I60" s="157"/>
-      <c r="J60" s="158"/>
+      <c r="J60" s="158" t="str">
+        <f t="shared" si="24"/>
+        <v>0x00</v>
+      </c>
       <c r="U60" s="153" t="s">
         <v>661</v>
       </c>
@@ -11063,7 +11081,7 @@
       </c>
     </row>
     <row r="61" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B61" s="215"/>
+      <c r="B61" s="211"/>
       <c r="C61" s="31" t="s">
         <v>431</v>
       </c>
@@ -11077,7 +11095,10 @@
       </c>
       <c r="H61" s="157"/>
       <c r="I61" s="157"/>
-      <c r="J61" s="158"/>
+      <c r="J61" s="158" t="str">
+        <f t="shared" si="24"/>
+        <v>0x00</v>
+      </c>
       <c r="U61" s="153" t="s">
         <v>664</v>
       </c>
@@ -11086,7 +11107,7 @@
       </c>
     </row>
     <row r="62" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B62" s="215"/>
+      <c r="B62" s="211"/>
       <c r="C62" s="31" t="s">
         <v>433</v>
       </c>
@@ -11095,10 +11116,15 @@
       </c>
       <c r="E62" s="166"/>
       <c r="F62" s="166"/>
-      <c r="G62" s="166"/>
+      <c r="G62" s="165" t="s">
+        <v>794</v>
+      </c>
       <c r="H62" s="157"/>
       <c r="I62" s="157"/>
-      <c r="J62" s="158"/>
+      <c r="J62" s="158" t="str">
+        <f t="shared" si="24"/>
+        <v>0xFF</v>
+      </c>
       <c r="U62" s="153" t="s">
         <v>668</v>
       </c>
@@ -11107,7 +11133,7 @@
       </c>
     </row>
     <row r="63" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="216"/>
+      <c r="B63" s="212"/>
       <c r="C63" s="35" t="s">
         <v>434</v>
       </c>
@@ -11121,7 +11147,10 @@
       </c>
       <c r="H63" s="162"/>
       <c r="I63" s="162"/>
-      <c r="J63" s="163"/>
+      <c r="J63" s="163" t="str">
+        <f t="shared" si="24"/>
+        <v>0x00</v>
+      </c>
       <c r="U63" s="153" t="s">
         <v>665</v>
       </c>
@@ -11130,7 +11159,7 @@
       </c>
     </row>
     <row r="64" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B64" s="214">
+      <c r="B64" s="210">
         <v>6</v>
       </c>
       <c r="C64" s="28" t="s">
@@ -11158,8 +11187,8 @@
         <v>561</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="215"/>
+    <row r="65" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B65" s="211"/>
       <c r="C65" s="31" t="s">
         <v>424</v>
       </c>
@@ -11188,8 +11217,8 @@
         <v>0x03</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="215"/>
+    <row r="66" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B66" s="211"/>
       <c r="C66" s="31" t="s">
         <v>425</v>
       </c>
@@ -11218,8 +11247,8 @@
         <v>0x03</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="215"/>
+    <row r="67" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B67" s="211"/>
       <c r="C67" s="31" t="s">
         <v>426</v>
       </c>
@@ -11248,8 +11277,8 @@
         <v>0x03</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="215"/>
+    <row r="68" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B68" s="211"/>
       <c r="C68" s="81" t="s">
         <v>427</v>
       </c>
@@ -11278,8 +11307,8 @@
         <v>0x03</v>
       </c>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" s="215"/>
+    <row r="69" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B69" s="211"/>
       <c r="C69" s="31" t="s">
         <v>428</v>
       </c>
@@ -11305,8 +11334,8 @@
         <v>777</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" s="215"/>
+    <row r="70" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B70" s="211"/>
       <c r="C70" s="31" t="s">
         <v>429</v>
       </c>
@@ -11322,8 +11351,8 @@
       <c r="I70" s="157"/>
       <c r="J70" s="158"/>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" s="215"/>
+    <row r="71" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B71" s="211"/>
       <c r="C71" s="81" t="s">
         <v>430</v>
       </c>
@@ -11339,8 +11368,8 @@
       <c r="I71" s="157"/>
       <c r="J71" s="158"/>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" s="215"/>
+    <row r="72" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B72" s="211"/>
       <c r="C72" s="31" t="s">
         <v>431</v>
       </c>
@@ -11356,8 +11385,8 @@
       <c r="I72" s="157"/>
       <c r="J72" s="158"/>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" s="215"/>
+    <row r="73" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B73" s="211"/>
       <c r="C73" s="31" t="s">
         <v>433</v>
       </c>
@@ -11373,8 +11402,8 @@
       <c r="I73" s="157"/>
       <c r="J73" s="158"/>
     </row>
-    <row r="74" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="216"/>
+    <row r="74" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="212"/>
       <c r="C74" s="35" t="s">
         <v>434</v>
       </c>
@@ -11390,13 +11419,294 @@
       <c r="I74" s="162"/>
       <c r="J74" s="163"/>
     </row>
+    <row r="75" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B75" s="210">
+        <v>7</v>
+      </c>
+      <c r="C75" s="28" t="s">
+        <v>648</v>
+      </c>
+      <c r="D75" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="E75" s="164" t="s">
+        <v>559</v>
+      </c>
+      <c r="F75" s="164" t="s">
+        <v>560</v>
+      </c>
+      <c r="G75" s="164" t="s">
+        <v>561</v>
+      </c>
+      <c r="H75" s="155" t="s">
+        <v>559</v>
+      </c>
+      <c r="I75" s="155" t="s">
+        <v>560</v>
+      </c>
+      <c r="J75" s="156" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="76" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B76" s="211"/>
+      <c r="C76" s="31" t="s">
+        <v>424</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E76" s="166" t="s">
+        <v>733</v>
+      </c>
+      <c r="F76" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G76" s="165" t="s">
+        <v>581</v>
+      </c>
+      <c r="H76" s="157" t="str">
+        <f t="shared" ref="H76:H79" si="31">CONCATENATE("0x",BIN2HEX(RIGHT(E76,LEN(E76)-2),2))</f>
+        <v>0x0E</v>
+      </c>
+      <c r="I76" s="157" t="str">
+        <f t="shared" ref="I76:I79" si="32">CONCATENATE("0x",BIN2HEX(RIGHT(F76,LEN(F76)-2),2))</f>
+        <v>0x40</v>
+      </c>
+      <c r="J76" s="158" t="str">
+        <f t="shared" ref="J76:J79" si="33">CONCATENATE("0x",BIN2HEX(RIGHT(G76,LEN(G76)-2),2))</f>
+        <v>0x03</v>
+      </c>
+      <c r="K76" s="161" t="s">
+        <v>705</v>
+      </c>
+      <c r="L76" s="11" t="str">
+        <f t="shared" ref="L76" si="34">INDEX($V$18:$V$25,MATCH(LEFT(RIGHT(E76,LEN(E76)-2-3),3),$U$18:$U$25,0))</f>
+        <v>7k</v>
+      </c>
+      <c r="M76" s="11" t="str">
+        <f t="shared" ref="M76" si="35">INDEX($V$27:$V$30,MATCH(LEFT(RIGHT(E76,LEN(E76)-2-6),2),$U$27:$U$30,0))</f>
+        <v>50R</v>
+      </c>
+      <c r="N76" s="11" t="str">
+        <f t="shared" ref="N76" si="36">INDEX($V$32:$V$33,MATCH(LEFT(RIGHT(F76,LEN(F76)-2),1),$U$32:$U$33,0))</f>
+        <v>VDD</v>
+      </c>
+      <c r="O76" s="11" t="str">
+        <f t="shared" ref="O76" si="37">INDEX($V$35:$V$38,MATCH(LEFT(RIGHT(F76,LEN(F76)-2-1),2),$U$35:$U$38,0))</f>
+        <v>67%</v>
+      </c>
+      <c r="P76" s="11" t="str">
+        <f t="shared" ref="P76" si="38">INDEX($V$40:$V$41,MATCH(LEFT(RIGHT(F76,LEN(F76)-2-3),1),$U$40:$U$41,0))</f>
+        <v>NEG</v>
+      </c>
+      <c r="Q76" s="154">
+        <f t="shared" ref="Q76" si="39">INDEX($V$43:$V$56,MATCH(LEFT(RIGHT(F76,LEN(F76)-2-4),4),$U$43:$U$56,0))</f>
+        <v>0</v>
+      </c>
+      <c r="R76" s="11" t="str">
+        <f t="shared" ref="R76" si="40">INDEX($V$58:$V$63,MATCH(LEFT(RIGHT(G76,LEN(G76)-2-5),3),$U$58:$U$63,0))</f>
+        <v>3-lead amperometric</v>
+      </c>
+      <c r="S76" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="77" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B77" s="211"/>
+      <c r="C77" s="31" t="s">
+        <v>425</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E77" s="166" t="s">
+        <v>733</v>
+      </c>
+      <c r="F77" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G77" s="165" t="s">
+        <v>581</v>
+      </c>
+      <c r="H77" s="157" t="str">
+        <f t="shared" si="31"/>
+        <v>0x0E</v>
+      </c>
+      <c r="I77" s="157" t="str">
+        <f t="shared" si="32"/>
+        <v>0x40</v>
+      </c>
+      <c r="J77" s="158" t="str">
+        <f t="shared" si="33"/>
+        <v>0x03</v>
+      </c>
+    </row>
+    <row r="78" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B78" s="211"/>
+      <c r="C78" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E78" s="166" t="s">
+        <v>733</v>
+      </c>
+      <c r="F78" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G78" s="165" t="s">
+        <v>581</v>
+      </c>
+      <c r="H78" s="157" t="str">
+        <f t="shared" si="31"/>
+        <v>0x0E</v>
+      </c>
+      <c r="I78" s="157" t="str">
+        <f t="shared" si="32"/>
+        <v>0x40</v>
+      </c>
+      <c r="J78" s="158" t="str">
+        <f t="shared" si="33"/>
+        <v>0x03</v>
+      </c>
+    </row>
+    <row r="79" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B79" s="211"/>
+      <c r="C79" s="81" t="s">
+        <v>427</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E79" s="166" t="s">
+        <v>733</v>
+      </c>
+      <c r="F79" s="166" t="s">
+        <v>563</v>
+      </c>
+      <c r="G79" s="165" t="s">
+        <v>581</v>
+      </c>
+      <c r="H79" s="157" t="str">
+        <f t="shared" si="31"/>
+        <v>0x0E</v>
+      </c>
+      <c r="I79" s="157" t="str">
+        <f t="shared" si="32"/>
+        <v>0x40</v>
+      </c>
+      <c r="J79" s="158" t="str">
+        <f t="shared" si="33"/>
+        <v>0x03</v>
+      </c>
+    </row>
+    <row r="80" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B80" s="211"/>
+      <c r="C80" s="31" t="s">
+        <v>428</v>
+      </c>
+      <c r="D80" s="87" t="s">
+        <v>757</v>
+      </c>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="165" t="s">
+        <v>562</v>
+      </c>
+      <c r="H80" s="157"/>
+      <c r="I80" s="157"/>
+      <c r="J80" s="158"/>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B81" s="211"/>
+      <c r="C81" s="31" t="s">
+        <v>429</v>
+      </c>
+      <c r="D81" s="87" t="s">
+        <v>757</v>
+      </c>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="165" t="s">
+        <v>562</v>
+      </c>
+      <c r="H81" s="157"/>
+      <c r="I81" s="157"/>
+      <c r="J81" s="158"/>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B82" s="211"/>
+      <c r="C82" s="81" t="s">
+        <v>430</v>
+      </c>
+      <c r="D82" s="87" t="s">
+        <v>757</v>
+      </c>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="165" t="s">
+        <v>562</v>
+      </c>
+      <c r="H82" s="157"/>
+      <c r="I82" s="157"/>
+      <c r="J82" s="158"/>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B83" s="211"/>
+      <c r="C83" s="31" t="s">
+        <v>431</v>
+      </c>
+      <c r="D83" s="87" t="s">
+        <v>757</v>
+      </c>
+      <c r="E83" s="137"/>
+      <c r="F83" s="137"/>
+      <c r="G83" s="165" t="s">
+        <v>562</v>
+      </c>
+      <c r="H83" s="157"/>
+      <c r="I83" s="157"/>
+      <c r="J83" s="158"/>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B84" s="211"/>
+      <c r="C84" s="31" t="s">
+        <v>433</v>
+      </c>
+      <c r="D84" s="87" t="s">
+        <v>757</v>
+      </c>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="165" t="s">
+        <v>562</v>
+      </c>
+      <c r="H84" s="157"/>
+      <c r="I84" s="157"/>
+      <c r="J84" s="158"/>
+    </row>
+    <row r="85" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="212"/>
+      <c r="C85" s="35" t="s">
+        <v>434</v>
+      </c>
+      <c r="D85" s="35" t="s">
+        <v>757</v>
+      </c>
+      <c r="E85" s="193"/>
+      <c r="F85" s="193"/>
+      <c r="G85" s="194" t="s">
+        <v>562</v>
+      </c>
+      <c r="H85" s="162"/>
+      <c r="I85" s="162"/>
+      <c r="J85" s="163"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B64:B74"/>
-    <mergeCell ref="B31:B41"/>
-    <mergeCell ref="B42:B52"/>
-    <mergeCell ref="B53:B63"/>
-    <mergeCell ref="U16:V16"/>
+  <mergeCells count="14">
+    <mergeCell ref="B75:B85"/>
     <mergeCell ref="E15:G15"/>
     <mergeCell ref="L15:R15"/>
     <mergeCell ref="B20:B30"/>
@@ -11405,6 +11715,11 @@
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:J12"/>
     <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B64:B74"/>
+    <mergeCell ref="B31:B41"/>
+    <mergeCell ref="B42:B52"/>
+    <mergeCell ref="B53:B63"/>
+    <mergeCell ref="U16:V16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B1" location="Contents!A1" display="Contents!A1"/>
@@ -14535,7 +14850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>